<commit_message>
add plan data file
</commit_message>
<xml_diff>
--- a/Data/UCRP-MembersData-2015.xlsx
+++ b/Data/UCRP-MembersData-2015.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="24900" firstSheet="7" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="24900" firstSheet="8" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Data_Doc" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="825" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="828" uniqueCount="107">
   <si>
     <t>&lt; 50</t>
   </si>
@@ -337,6 +337,24 @@
   </si>
   <si>
     <t>10-14</t>
+  </si>
+  <si>
+    <t>20+</t>
+  </si>
+  <si>
+    <t>5-10</t>
+  </si>
+  <si>
+    <t>11-20</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>13Tier</t>
+  </si>
+  <si>
+    <t>76Tier</t>
   </si>
 </sst>
 </file>
@@ -513,7 +531,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -659,6 +677,12 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1008,7 +1032,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1045,14 +1069,14 @@
       <c r="B4" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="C4" s="36" t="s">
-        <v>49</v>
-      </c>
-      <c r="D4" s="36" t="s">
-        <v>50</v>
+      <c r="C4" s="54" t="s">
+        <v>102</v>
+      </c>
+      <c r="D4" s="54" t="s">
+        <v>103</v>
       </c>
       <c r="E4" s="36" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1214,8 +1238,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1351,8 +1375,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1489,7 +1513,7 @@
   <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A29" sqref="A29:K31"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7110,10 +7134,13 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G64" sqref="G64"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
@@ -7128,16 +7155,16 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
-        <v>60</v>
+        <v>104</v>
       </c>
       <c r="B2" s="35" t="s">
         <v>59</v>
       </c>
       <c r="C2" s="36" t="s">
-        <v>5</v>
+        <v>105</v>
       </c>
       <c r="D2" s="36" t="s">
-        <v>6</v>
+        <v>106</v>
       </c>
       <c r="E2" s="36" t="s">
         <v>7</v>
@@ -7150,7 +7177,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="46" t="s">
+      <c r="A3" s="28" t="s">
         <v>65</v>
       </c>
       <c r="B3" s="6" t="s">
@@ -7173,7 +7200,9 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="46"/>
+      <c r="A4" s="28" t="s">
+        <v>65</v>
+      </c>
       <c r="B4" s="6" t="s">
         <v>12</v>
       </c>
@@ -7194,7 +7223,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="46" t="s">
+      <c r="A5" s="28" t="s">
         <v>13</v>
       </c>
       <c r="B5" s="6" t="s">
@@ -7217,7 +7246,9 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="46"/>
+      <c r="A6" s="28" t="s">
+        <v>13</v>
+      </c>
       <c r="B6" s="6" t="s">
         <v>12</v>
       </c>
@@ -7238,7 +7269,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="46" t="s">
+      <c r="A7" s="28" t="s">
         <v>14</v>
       </c>
       <c r="B7" s="6" t="s">
@@ -7261,7 +7292,9 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="46"/>
+      <c r="A8" s="28" t="s">
+        <v>14</v>
+      </c>
       <c r="B8" s="6" t="s">
         <v>12</v>
       </c>
@@ -7282,11 +7315,6 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A7:A8"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -7695,7 +7723,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F65" sqref="F65"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7753,14 +7781,14 @@
       <c r="B6" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="C6" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>50</v>
+      <c r="C6" s="55" t="s">
+        <v>102</v>
+      </c>
+      <c r="D6" s="55" t="s">
+        <v>103</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="F6" s="35" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
script for initial terms
</commit_message>
<xml_diff>
--- a/Data/UCRP-MembersData-2015.xlsx
+++ b/Data/UCRP-MembersData-2015.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="24900" firstSheet="8" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="24900" firstSheet="8" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Data_Doc" sheetId="2" r:id="rId1"/>
@@ -654,6 +654,12 @@
     <xf numFmtId="16" fontId="8" fillId="3" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -677,12 +683,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1031,7 +1031,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
@@ -1055,12 +1055,12 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="22"/>
-      <c r="B3" s="47" t="s">
+      <c r="B3" s="49" t="s">
         <v>48</v>
       </c>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
     </row>
     <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="34" t="s">
@@ -1069,10 +1069,10 @@
       <c r="B4" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="C4" s="54" t="s">
+      <c r="C4" s="46" t="s">
         <v>102</v>
       </c>
-      <c r="D4" s="54" t="s">
+      <c r="D4" s="46" t="s">
         <v>103</v>
       </c>
       <c r="E4" s="36" t="s">
@@ -1375,7 +1375,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
@@ -1539,25 +1539,25 @@
       <c r="K1" s="38"/>
     </row>
     <row r="2" spans="1:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="50" t="s">
         <v>73</v>
       </c>
-      <c r="B2" s="49"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="50"/>
+      <c r="B2" s="51"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="52"/>
       <c r="I2" s="37"/>
       <c r="J2" s="37"/>
       <c r="K2" s="37"/>
     </row>
     <row r="3" spans="1:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="53" t="s">
         <v>74</v>
       </c>
-      <c r="B3" s="52"/>
+      <c r="B3" s="54"/>
       <c r="C3" s="38"/>
       <c r="D3" s="38"/>
       <c r="E3" s="38"/>
@@ -1569,14 +1569,14 @@
       <c r="K3" s="38"/>
     </row>
     <row r="4" spans="1:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="48" t="s">
+      <c r="A4" s="50" t="s">
         <v>94</v>
       </c>
-      <c r="B4" s="49"/>
-      <c r="C4" s="49"/>
-      <c r="D4" s="49"/>
-      <c r="E4" s="49"/>
-      <c r="F4" s="50"/>
+      <c r="B4" s="51"/>
+      <c r="C4" s="51"/>
+      <c r="D4" s="51"/>
+      <c r="E4" s="51"/>
+      <c r="F4" s="52"/>
       <c r="G4" s="37"/>
       <c r="H4" s="37"/>
       <c r="I4" s="37"/>
@@ -1589,10 +1589,10 @@
       <c r="C5" s="38"/>
       <c r="D5" s="38"/>
       <c r="E5" s="38"/>
-      <c r="F5" s="51" t="s">
+      <c r="F5" s="53" t="s">
         <v>48</v>
       </c>
-      <c r="G5" s="52"/>
+      <c r="G5" s="54"/>
       <c r="H5" s="38"/>
       <c r="I5" s="38"/>
       <c r="J5" s="38"/>
@@ -2481,17 +2481,17 @@
       <c r="A1" s="37" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="50" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
-      <c r="H1" s="49"/>
-      <c r="I1" s="49"/>
-      <c r="J1" s="50"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="51"/>
+      <c r="I1" s="51"/>
+      <c r="J1" s="52"/>
       <c r="K1" s="37"/>
     </row>
     <row r="2" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2510,26 +2510,26 @@
       <c r="K2" s="38"/>
     </row>
     <row r="3" spans="1:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="50" t="s">
         <v>73</v>
       </c>
-      <c r="B3" s="49"/>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="49"/>
-      <c r="F3" s="49"/>
-      <c r="G3" s="49"/>
-      <c r="H3" s="50"/>
+      <c r="B3" s="51"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="52"/>
       <c r="I3" s="37"/>
       <c r="J3" s="37"/>
       <c r="K3" s="37"/>
     </row>
     <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="51" t="s">
+      <c r="A4" s="53" t="s">
         <v>74</v>
       </c>
-      <c r="B4" s="53"/>
-      <c r="C4" s="52"/>
+      <c r="B4" s="55"/>
+      <c r="C4" s="54"/>
       <c r="D4" s="38"/>
       <c r="E4" s="38"/>
       <c r="F4" s="38"/>
@@ -2540,18 +2540,18 @@
       <c r="K4" s="38"/>
     </row>
     <row r="5" spans="1:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="48" t="s">
+      <c r="A5" s="50" t="s">
         <v>95</v>
       </c>
-      <c r="B5" s="49"/>
-      <c r="C5" s="49"/>
-      <c r="D5" s="49"/>
-      <c r="E5" s="49"/>
-      <c r="F5" s="49"/>
-      <c r="G5" s="49"/>
-      <c r="H5" s="49"/>
-      <c r="I5" s="49"/>
-      <c r="J5" s="50"/>
+      <c r="B5" s="51"/>
+      <c r="C5" s="51"/>
+      <c r="D5" s="51"/>
+      <c r="E5" s="51"/>
+      <c r="F5" s="51"/>
+      <c r="G5" s="51"/>
+      <c r="H5" s="51"/>
+      <c r="I5" s="51"/>
+      <c r="J5" s="52"/>
       <c r="K5" s="37"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2560,10 +2560,10 @@
       <c r="C6" s="38"/>
       <c r="D6" s="38"/>
       <c r="E6" s="38"/>
-      <c r="F6" s="51" t="s">
+      <c r="F6" s="53" t="s">
         <v>48</v>
       </c>
-      <c r="G6" s="52"/>
+      <c r="G6" s="54"/>
       <c r="H6" s="38"/>
       <c r="I6" s="38"/>
       <c r="J6" s="38"/>
@@ -3452,17 +3452,17 @@
       <c r="A1" s="37" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="50" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
-      <c r="H1" s="49"/>
-      <c r="I1" s="49"/>
-      <c r="J1" s="50"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="51"/>
+      <c r="I1" s="51"/>
+      <c r="J1" s="52"/>
       <c r="K1" s="37"/>
     </row>
     <row r="2" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3481,26 +3481,26 @@
       <c r="K2" s="38"/>
     </row>
     <row r="3" spans="1:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="50" t="s">
         <v>73</v>
       </c>
-      <c r="B3" s="49"/>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="49"/>
-      <c r="F3" s="49"/>
-      <c r="G3" s="49"/>
-      <c r="H3" s="50"/>
+      <c r="B3" s="51"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="52"/>
       <c r="I3" s="37"/>
       <c r="J3" s="37"/>
       <c r="K3" s="37"/>
     </row>
     <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="51" t="s">
+      <c r="A4" s="53" t="s">
         <v>74</v>
       </c>
-      <c r="B4" s="53"/>
-      <c r="C4" s="52"/>
+      <c r="B4" s="55"/>
+      <c r="C4" s="54"/>
       <c r="D4" s="38"/>
       <c r="E4" s="38"/>
       <c r="F4" s="38"/>
@@ -3511,18 +3511,18 @@
       <c r="K4" s="38"/>
     </row>
     <row r="5" spans="1:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="48" t="s">
+      <c r="A5" s="50" t="s">
         <v>96</v>
       </c>
-      <c r="B5" s="49"/>
-      <c r="C5" s="49"/>
-      <c r="D5" s="49"/>
-      <c r="E5" s="49"/>
-      <c r="F5" s="49"/>
-      <c r="G5" s="49"/>
-      <c r="H5" s="49"/>
-      <c r="I5" s="49"/>
-      <c r="J5" s="50"/>
+      <c r="B5" s="51"/>
+      <c r="C5" s="51"/>
+      <c r="D5" s="51"/>
+      <c r="E5" s="51"/>
+      <c r="F5" s="51"/>
+      <c r="G5" s="51"/>
+      <c r="H5" s="51"/>
+      <c r="I5" s="51"/>
+      <c r="J5" s="52"/>
       <c r="K5" s="37"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3546,10 +3546,10 @@
       <c r="C7" s="37"/>
       <c r="D7" s="37"/>
       <c r="E7" s="37"/>
-      <c r="F7" s="48" t="s">
+      <c r="F7" s="50" t="s">
         <v>48</v>
       </c>
-      <c r="G7" s="50"/>
+      <c r="G7" s="52"/>
       <c r="H7" s="37"/>
       <c r="I7" s="37"/>
       <c r="J7" s="37"/>
@@ -4440,17 +4440,17 @@
       <c r="A1" s="37" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="50" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
-      <c r="H1" s="49"/>
-      <c r="I1" s="49"/>
-      <c r="J1" s="50"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="51"/>
+      <c r="I1" s="51"/>
+      <c r="J1" s="52"/>
       <c r="K1" s="37"/>
     </row>
     <row r="2" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4469,25 +4469,25 @@
       <c r="K2" s="38"/>
     </row>
     <row r="3" spans="1:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="50" t="s">
         <v>73</v>
       </c>
-      <c r="B3" s="49"/>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="49"/>
-      <c r="F3" s="49"/>
-      <c r="G3" s="49"/>
-      <c r="H3" s="50"/>
+      <c r="B3" s="51"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="52"/>
       <c r="I3" s="37"/>
       <c r="J3" s="37"/>
       <c r="K3" s="37"/>
     </row>
     <row r="4" spans="1:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="51" t="s">
+      <c r="A4" s="53" t="s">
         <v>74</v>
       </c>
-      <c r="B4" s="52"/>
+      <c r="B4" s="54"/>
       <c r="C4" s="38"/>
       <c r="D4" s="38"/>
       <c r="E4" s="38"/>
@@ -4499,10 +4499,10 @@
       <c r="K4" s="38"/>
     </row>
     <row r="5" spans="1:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="48" t="s">
+      <c r="A5" s="50" t="s">
         <v>98</v>
       </c>
-      <c r="B5" s="50"/>
+      <c r="B5" s="52"/>
       <c r="C5" s="37"/>
       <c r="D5" s="37"/>
       <c r="E5" s="37"/>
@@ -4519,10 +4519,10 @@
       <c r="C6" s="38"/>
       <c r="D6" s="38"/>
       <c r="E6" s="38"/>
-      <c r="F6" s="51" t="s">
+      <c r="F6" s="53" t="s">
         <v>48</v>
       </c>
-      <c r="G6" s="52"/>
+      <c r="G6" s="54"/>
       <c r="H6" s="38"/>
       <c r="I6" s="38"/>
       <c r="J6" s="38"/>
@@ -5771,12 +5771,12 @@
     </row>
     <row r="35" spans="1:6" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
-      <c r="B35" s="47" t="s">
+      <c r="B35" s="49" t="s">
         <v>48</v>
       </c>
-      <c r="C35" s="47"/>
-      <c r="D35" s="47"/>
-      <c r="E35" s="47"/>
+      <c r="C35" s="49"/>
+      <c r="D35" s="49"/>
+      <c r="E35" s="49"/>
     </row>
     <row r="36" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
@@ -6008,12 +6008,12 @@
     </row>
     <row r="51" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="22"/>
-      <c r="B51" s="47" t="s">
+      <c r="B51" s="49" t="s">
         <v>48</v>
       </c>
-      <c r="C51" s="47"/>
-      <c r="D51" s="47"/>
-      <c r="E51" s="47"/>
+      <c r="C51" s="49"/>
+      <c r="D51" s="49"/>
+      <c r="E51" s="49"/>
     </row>
     <row r="52" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
@@ -6203,12 +6203,12 @@
     </row>
     <row r="68" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="22"/>
-      <c r="B68" s="47" t="s">
+      <c r="B68" s="49" t="s">
         <v>48</v>
       </c>
-      <c r="C68" s="47"/>
-      <c r="D68" s="47"/>
-      <c r="E68" s="47"/>
+      <c r="C68" s="49"/>
+      <c r="D68" s="49"/>
+      <c r="E68" s="49"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
@@ -6317,12 +6317,12 @@
     </row>
     <row r="78" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="4"/>
-      <c r="B78" s="47" t="s">
+      <c r="B78" s="49" t="s">
         <v>48</v>
       </c>
-      <c r="C78" s="47"/>
-      <c r="D78" s="47"/>
-      <c r="E78" s="47"/>
+      <c r="C78" s="49"/>
+      <c r="D78" s="49"/>
+      <c r="E78" s="49"/>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="17" t="s">
@@ -6574,7 +6574,7 @@
       <c r="J101" s="12"/>
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A102" s="46" t="s">
+      <c r="A102" s="48" t="s">
         <v>65</v>
       </c>
       <c r="B102" s="6" t="s">
@@ -6600,7 +6600,7 @@
       <c r="J102" s="12"/>
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A103" s="46"/>
+      <c r="A103" s="48"/>
       <c r="B103" s="6" t="s">
         <v>12</v>
       </c>
@@ -6624,7 +6624,7 @@
       <c r="J103" s="12"/>
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A104" s="46" t="s">
+      <c r="A104" s="48" t="s">
         <v>13</v>
       </c>
       <c r="B104" s="6" t="s">
@@ -6650,7 +6650,7 @@
       <c r="J104" s="12"/>
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A105" s="46"/>
+      <c r="A105" s="48"/>
       <c r="B105" s="6" t="s">
         <v>12</v>
       </c>
@@ -6674,7 +6674,7 @@
       <c r="J105" s="12"/>
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A106" s="46" t="s">
+      <c r="A106" s="48" t="s">
         <v>14</v>
       </c>
       <c r="B106" s="6" t="s">
@@ -6700,7 +6700,7 @@
       <c r="J106" s="12"/>
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A107" s="46"/>
+      <c r="A107" s="48"/>
       <c r="B107" s="6" t="s">
         <v>12</v>
       </c>
@@ -7451,12 +7451,12 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
-      <c r="B3" s="47" t="s">
+      <c r="B3" s="49" t="s">
         <v>48</v>
       </c>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="35" t="s">
@@ -7603,12 +7603,12 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="22"/>
-      <c r="B4" s="47" t="s">
+      <c r="B4" s="49" t="s">
         <v>48</v>
       </c>
-      <c r="C4" s="47"/>
-      <c r="D4" s="47"/>
-      <c r="E4" s="47"/>
+      <c r="C4" s="49"/>
+      <c r="D4" s="49"/>
+      <c r="E4" s="49"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="34" t="s">
@@ -7766,12 +7766,12 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
-      <c r="B5" s="47" t="s">
+      <c r="B5" s="49" t="s">
         <v>48</v>
       </c>
-      <c r="C5" s="47"/>
-      <c r="D5" s="47"/>
-      <c r="E5" s="47"/>
+      <c r="C5" s="49"/>
+      <c r="D5" s="49"/>
+      <c r="E5" s="49"/>
       <c r="F5" s="9"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -7781,10 +7781,10 @@
       <c r="B6" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="C6" s="55" t="s">
+      <c r="C6" s="47" t="s">
         <v>102</v>
       </c>
-      <c r="D6" s="55" t="s">
+      <c r="D6" s="47" t="s">
         <v>103</v>
       </c>
       <c r="E6" s="7" t="s">

</xml_diff>

<commit_message>
fixed a bug in salary
</commit_message>
<xml_diff>
--- a/Data/UCRP-MembersData-2015.xlsx
+++ b/Data/UCRP-MembersData-2015.xlsx
@@ -9,32 +9,33 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="24900" firstSheet="8" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="24900"/>
   </bookViews>
   <sheets>
-    <sheet name="Data_Doc" sheetId="2" r:id="rId1"/>
-    <sheet name="2015" sheetId="4" r:id="rId2"/>
-    <sheet name="Sum_Disabled" sheetId="19" r:id="rId3"/>
-    <sheet name="Sum_Retirees" sheetId="20" r:id="rId4"/>
-    <sheet name="Sum_Active" sheetId="18" r:id="rId5"/>
-    <sheet name="CAP" sheetId="17" r:id="rId6"/>
-    <sheet name="Disabled_Inc" sheetId="15" r:id="rId7"/>
-    <sheet name="Disabled_HAPC" sheetId="16" r:id="rId8"/>
-    <sheet name="Terms_N" sheetId="13" r:id="rId9"/>
-    <sheet name="Terms_HAPC" sheetId="14" r:id="rId10"/>
-    <sheet name="Retirees" sheetId="11" r:id="rId11"/>
-    <sheet name="Beneficiaries" sheetId="12" r:id="rId12"/>
-    <sheet name="Active_t76" sheetId="7" r:id="rId13"/>
-    <sheet name="Active_t13" sheetId="8" r:id="rId14"/>
-    <sheet name="Active_tm13" sheetId="9" r:id="rId15"/>
-    <sheet name="Active_safety" sheetId="10" r:id="rId16"/>
+    <sheet name="Active_t76 (2)" sheetId="21" r:id="rId1"/>
+    <sheet name="Data_Doc" sheetId="2" r:id="rId2"/>
+    <sheet name="2015" sheetId="4" r:id="rId3"/>
+    <sheet name="Sum_Disabled" sheetId="19" r:id="rId4"/>
+    <sheet name="Sum_Retirees" sheetId="20" r:id="rId5"/>
+    <sheet name="Sum_Active" sheetId="18" r:id="rId6"/>
+    <sheet name="CAP" sheetId="17" r:id="rId7"/>
+    <sheet name="Disabled_Inc" sheetId="15" r:id="rId8"/>
+    <sheet name="Disabled_HAPC" sheetId="16" r:id="rId9"/>
+    <sheet name="Terms_N" sheetId="13" r:id="rId10"/>
+    <sheet name="Terms_HAPC" sheetId="14" r:id="rId11"/>
+    <sheet name="Retirees" sheetId="11" r:id="rId12"/>
+    <sheet name="Beneficiaries" sheetId="12" r:id="rId13"/>
+    <sheet name="Active_t76" sheetId="7" r:id="rId14"/>
+    <sheet name="Active_t13" sheetId="8" r:id="rId15"/>
+    <sheet name="Active_tm13" sheetId="9" r:id="rId16"/>
+    <sheet name="Active_safety" sheetId="10" r:id="rId17"/>
   </sheets>
   <calcPr calcId="162913" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="828" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="911" uniqueCount="107">
   <si>
     <t>&lt; 50</t>
   </si>
@@ -531,7 +532,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -660,6 +661,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -684,6 +688,7 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -988,46 +993,1563 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:A9"/>
+  <dimension ref="A1:K43"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="7" width="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="27.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="38" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+    </row>
+    <row r="2" spans="1:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="51" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+    </row>
+    <row r="3" spans="1:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="48" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
+    </row>
+    <row r="4" spans="1:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="51" t="s">
+        <v>94</v>
+      </c>
+      <c r="B4" s="52"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="53"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="37"/>
+      <c r="I4" s="37"/>
+      <c r="J4" s="37"/>
+    </row>
+    <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="38"/>
+      <c r="B5" s="38"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="54" t="s">
+        <v>48</v>
+      </c>
+      <c r="F5" s="55"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="38"/>
+      <c r="I5" s="38"/>
+      <c r="J5" s="38"/>
+    </row>
+    <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="37" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="39" t="s">
+        <v>75</v>
+      </c>
+      <c r="C6" s="45" t="s">
+        <v>99</v>
+      </c>
+      <c r="D6" s="45" t="s">
+        <v>100</v>
+      </c>
+      <c r="E6" s="39" t="s">
+        <v>76</v>
+      </c>
+      <c r="F6" s="39" t="s">
+        <v>77</v>
+      </c>
+      <c r="G6" s="39" t="s">
+        <v>78</v>
+      </c>
+      <c r="H6" s="39" t="s">
+        <v>79</v>
+      </c>
+      <c r="I6" s="39" t="s">
+        <v>80</v>
+      </c>
+      <c r="J6" s="37" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="38" t="s">
+        <v>82</v>
+      </c>
+      <c r="B7" s="41">
+        <v>450</v>
+      </c>
+      <c r="C7" s="41">
+        <v>16</v>
+      </c>
+      <c r="D7" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="E7" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="F7" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="G7" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="H7" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="I7" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="J7" s="41" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="37"/>
+      <c r="B8" s="42">
+        <v>49125</v>
+      </c>
+      <c r="C8" s="42">
+        <v>42899</v>
+      </c>
+      <c r="D8" s="39" t="s">
+        <v>83</v>
+      </c>
+      <c r="E8" s="39" t="s">
+        <v>83</v>
+      </c>
+      <c r="F8" s="39" t="s">
+        <v>83</v>
+      </c>
+      <c r="G8" s="39" t="s">
+        <v>83</v>
+      </c>
+      <c r="H8" s="39" t="s">
+        <v>83</v>
+      </c>
+      <c r="I8" s="39" t="s">
+        <v>83</v>
+      </c>
+      <c r="J8" s="39" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="37"/>
+      <c r="B9" s="42">
+        <f t="shared" ref="B9:C9" si="0">B7*B8</f>
+        <v>22106250</v>
+      </c>
+      <c r="C9" s="42">
+        <f t="shared" si="0"/>
+        <v>686384</v>
+      </c>
+      <c r="D9" s="39"/>
+      <c r="E9" s="39"/>
+      <c r="F9" s="39"/>
+      <c r="G9" s="39"/>
+      <c r="H9" s="39"/>
+      <c r="I9" s="39"/>
+      <c r="J9" s="39"/>
+      <c r="K9" s="57">
+        <f>SUM(B9:J9)</f>
+        <v>22792634</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="41" t="s">
+        <v>84</v>
+      </c>
+      <c r="B10" s="40">
+        <v>4091</v>
+      </c>
+      <c r="C10" s="40">
+        <v>1113</v>
+      </c>
+      <c r="D10" s="41">
+        <v>18</v>
+      </c>
+      <c r="E10" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="F10" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="G10" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="H10" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="I10" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="J10" s="41" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="37"/>
+      <c r="B11" s="43">
+        <v>62836</v>
+      </c>
+      <c r="C11" s="43">
+        <v>59637</v>
+      </c>
+      <c r="D11" s="42">
+        <v>46481</v>
+      </c>
+      <c r="E11" s="39" t="s">
+        <v>83</v>
+      </c>
+      <c r="F11" s="39" t="s">
+        <v>83</v>
+      </c>
+      <c r="G11" s="39" t="s">
+        <v>83</v>
+      </c>
+      <c r="H11" s="39" t="s">
+        <v>83</v>
+      </c>
+      <c r="I11" s="39" t="s">
+        <v>83</v>
+      </c>
+      <c r="J11" s="39" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="37"/>
+      <c r="B12" s="42">
+        <f t="shared" ref="B12:D12" si="1">B10*B11</f>
+        <v>257062076</v>
+      </c>
+      <c r="C12" s="42">
+        <f t="shared" si="1"/>
+        <v>66375981</v>
+      </c>
+      <c r="D12" s="42">
+        <f t="shared" si="1"/>
+        <v>836658</v>
+      </c>
+      <c r="E12" s="39"/>
+      <c r="F12" s="39"/>
+      <c r="G12" s="39"/>
+      <c r="H12" s="39"/>
+      <c r="I12" s="39"/>
+      <c r="J12" s="39"/>
+      <c r="K12" s="57">
+        <f>SUM(B12:J12)</f>
+        <v>324274715</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="41" t="s">
+        <v>85</v>
+      </c>
+      <c r="B13" s="40">
+        <v>4579</v>
+      </c>
+      <c r="C13" s="40">
+        <v>4661</v>
+      </c>
+      <c r="D13" s="41">
+        <v>744</v>
+      </c>
+      <c r="E13" s="41">
+        <v>20</v>
+      </c>
+      <c r="F13" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="G13" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="H13" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="I13" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="J13" s="41" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="37"/>
+      <c r="B14" s="43">
+        <v>77686</v>
+      </c>
+      <c r="C14" s="43">
+        <v>75964</v>
+      </c>
+      <c r="D14" s="43">
+        <v>66937</v>
+      </c>
+      <c r="E14" s="42">
+        <v>57202</v>
+      </c>
+      <c r="F14" s="39" t="s">
+        <v>83</v>
+      </c>
+      <c r="G14" s="39" t="s">
+        <v>83</v>
+      </c>
+      <c r="H14" s="39" t="s">
+        <v>83</v>
+      </c>
+      <c r="I14" s="39" t="s">
+        <v>83</v>
+      </c>
+      <c r="J14" s="39" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="37"/>
+      <c r="B15" s="42">
+        <f t="shared" ref="B15:E15" si="2">B13*B14</f>
+        <v>355724194</v>
+      </c>
+      <c r="C15" s="42">
+        <f t="shared" si="2"/>
+        <v>354068204</v>
+      </c>
+      <c r="D15" s="42">
+        <f t="shared" si="2"/>
+        <v>49801128</v>
+      </c>
+      <c r="E15" s="42">
+        <f t="shared" si="2"/>
+        <v>1144040</v>
+      </c>
+      <c r="F15" s="39"/>
+      <c r="G15" s="39"/>
+      <c r="H15" s="39"/>
+      <c r="I15" s="39"/>
+      <c r="J15" s="39"/>
+      <c r="K15" s="57">
+        <f>SUM(B15:J15)</f>
+        <v>760737566</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="41" t="s">
+        <v>86</v>
+      </c>
+      <c r="B16" s="40">
+        <v>4218</v>
+      </c>
+      <c r="C16" s="40">
+        <v>5198</v>
+      </c>
+      <c r="D16" s="40">
+        <v>2558</v>
+      </c>
+      <c r="E16" s="41">
+        <v>514</v>
+      </c>
+      <c r="F16" s="41">
+        <v>6</v>
+      </c>
+      <c r="G16" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="H16" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="I16" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="J16" s="41" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="37"/>
+      <c r="B17" s="43">
+        <v>88621</v>
+      </c>
+      <c r="C17" s="43">
+        <v>90614</v>
+      </c>
+      <c r="D17" s="43">
+        <v>80010</v>
+      </c>
+      <c r="E17" s="43">
+        <v>75111</v>
+      </c>
+      <c r="F17" s="42">
+        <v>77949</v>
+      </c>
+      <c r="G17" s="39" t="s">
+        <v>83</v>
+      </c>
+      <c r="H17" s="39" t="s">
+        <v>83</v>
+      </c>
+      <c r="I17" s="39" t="s">
+        <v>83</v>
+      </c>
+      <c r="J17" s="39" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="37"/>
+      <c r="B18" s="42">
+        <f t="shared" ref="B18:F18" si="3">B16*B17</f>
+        <v>373803378</v>
+      </c>
+      <c r="C18" s="42">
+        <f t="shared" si="3"/>
+        <v>471011572</v>
+      </c>
+      <c r="D18" s="42">
+        <f t="shared" si="3"/>
+        <v>204665580</v>
+      </c>
+      <c r="E18" s="42">
+        <f t="shared" si="3"/>
+        <v>38607054</v>
+      </c>
+      <c r="F18" s="42">
+        <f t="shared" si="3"/>
+        <v>467694</v>
+      </c>
+      <c r="G18" s="39"/>
+      <c r="H18" s="39"/>
+      <c r="I18" s="39"/>
+      <c r="J18" s="39"/>
+      <c r="K18" s="57">
+        <f>SUM(B18:J18)</f>
+        <v>1088555278</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="41" t="s">
+        <v>87</v>
+      </c>
+      <c r="B19" s="40">
+        <v>2898</v>
+      </c>
+      <c r="C19" s="40">
+        <v>5157</v>
+      </c>
+      <c r="D19" s="40">
+        <v>3656</v>
+      </c>
+      <c r="E19" s="40">
+        <v>1582</v>
+      </c>
+      <c r="F19" s="41">
+        <v>305</v>
+      </c>
+      <c r="G19" s="41">
+        <v>11</v>
+      </c>
+      <c r="H19" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="I19" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="J19" s="41" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="37"/>
+      <c r="B20" s="43">
+        <v>89793</v>
+      </c>
+      <c r="C20" s="43">
+        <v>96293</v>
+      </c>
+      <c r="D20" s="43">
+        <v>95348</v>
+      </c>
+      <c r="E20" s="43">
+        <v>85513</v>
+      </c>
+      <c r="F20" s="43">
+        <v>81725</v>
+      </c>
+      <c r="G20" s="42">
+        <v>78205</v>
+      </c>
+      <c r="H20" s="39" t="s">
+        <v>83</v>
+      </c>
+      <c r="I20" s="39" t="s">
+        <v>83</v>
+      </c>
+      <c r="J20" s="39" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="37"/>
+      <c r="B21" s="42">
+        <f t="shared" ref="B21:G21" si="4">B19*B20</f>
+        <v>260220114</v>
+      </c>
+      <c r="C21" s="42">
+        <f t="shared" si="4"/>
+        <v>496583001</v>
+      </c>
+      <c r="D21" s="42">
+        <f t="shared" si="4"/>
+        <v>348592288</v>
+      </c>
+      <c r="E21" s="42">
+        <f t="shared" si="4"/>
+        <v>135281566</v>
+      </c>
+      <c r="F21" s="42">
+        <f t="shared" si="4"/>
+        <v>24926125</v>
+      </c>
+      <c r="G21" s="42">
+        <f t="shared" si="4"/>
+        <v>860255</v>
+      </c>
+      <c r="H21" s="39"/>
+      <c r="I21" s="39"/>
+      <c r="J21" s="39"/>
+      <c r="K21" s="57">
+        <f>SUM(B21:J21)</f>
+        <v>1266463349</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="41" t="s">
+        <v>88</v>
+      </c>
+      <c r="B22" s="40">
+        <v>2059</v>
+      </c>
+      <c r="C22" s="40">
+        <v>3911</v>
+      </c>
+      <c r="D22" s="40">
+        <v>3872</v>
+      </c>
+      <c r="E22" s="40">
+        <v>2416</v>
+      </c>
+      <c r="F22" s="40">
+        <v>1031</v>
+      </c>
+      <c r="G22" s="41">
+        <v>345</v>
+      </c>
+      <c r="H22" s="41">
+        <v>11</v>
+      </c>
+      <c r="I22" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="J22" s="41" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="37"/>
+      <c r="B23" s="43">
+        <v>88555</v>
+      </c>
+      <c r="C23" s="43">
+        <v>92609</v>
+      </c>
+      <c r="D23" s="43">
+        <v>99988</v>
+      </c>
+      <c r="E23" s="43">
+        <v>101093</v>
+      </c>
+      <c r="F23" s="43">
+        <v>93091</v>
+      </c>
+      <c r="G23" s="43">
+        <v>82653</v>
+      </c>
+      <c r="H23" s="42">
+        <v>71252</v>
+      </c>
+      <c r="I23" s="39" t="s">
+        <v>83</v>
+      </c>
+      <c r="J23" s="39" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="37"/>
+      <c r="B24" s="42">
+        <f t="shared" ref="B24:H24" si="5">B22*B23</f>
+        <v>182334745</v>
+      </c>
+      <c r="C24" s="42">
+        <f t="shared" si="5"/>
+        <v>362193799</v>
+      </c>
+      <c r="D24" s="42">
+        <f t="shared" si="5"/>
+        <v>387153536</v>
+      </c>
+      <c r="E24" s="42">
+        <f t="shared" si="5"/>
+        <v>244240688</v>
+      </c>
+      <c r="F24" s="42">
+        <f t="shared" si="5"/>
+        <v>95976821</v>
+      </c>
+      <c r="G24" s="42">
+        <f t="shared" si="5"/>
+        <v>28515285</v>
+      </c>
+      <c r="H24" s="42">
+        <f t="shared" si="5"/>
+        <v>783772</v>
+      </c>
+      <c r="I24" s="39"/>
+      <c r="J24" s="39"/>
+      <c r="K24" s="57">
+        <f>SUM(B24:J24)</f>
+        <v>1301198646</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="B25" s="40">
+        <v>1645</v>
+      </c>
+      <c r="C25" s="40">
+        <v>3133</v>
+      </c>
+      <c r="D25" s="40">
+        <v>3383</v>
+      </c>
+      <c r="E25" s="40">
+        <v>2698</v>
+      </c>
+      <c r="F25" s="40">
+        <v>1870</v>
+      </c>
+      <c r="G25" s="40">
+        <v>1212</v>
+      </c>
+      <c r="H25" s="41">
+        <v>293</v>
+      </c>
+      <c r="I25" s="41">
+        <v>15</v>
+      </c>
+      <c r="J25" s="41" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="37"/>
+      <c r="B26" s="43">
+        <v>91738</v>
+      </c>
+      <c r="C26" s="43">
+        <v>88111</v>
+      </c>
+      <c r="D26" s="43">
+        <v>95216</v>
+      </c>
+      <c r="E26" s="43">
+        <v>106204</v>
+      </c>
+      <c r="F26" s="43">
+        <v>111107</v>
+      </c>
+      <c r="G26" s="43">
+        <v>92436</v>
+      </c>
+      <c r="H26" s="43">
+        <v>90617</v>
+      </c>
+      <c r="I26" s="42">
+        <v>84431</v>
+      </c>
+      <c r="J26" s="39" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="37"/>
+      <c r="B27" s="42">
+        <f t="shared" ref="B27:I27" si="6">B25*B26</f>
+        <v>150909010</v>
+      </c>
+      <c r="C27" s="42">
+        <f t="shared" si="6"/>
+        <v>276051763</v>
+      </c>
+      <c r="D27" s="42">
+        <f t="shared" si="6"/>
+        <v>322115728</v>
+      </c>
+      <c r="E27" s="42">
+        <f t="shared" si="6"/>
+        <v>286538392</v>
+      </c>
+      <c r="F27" s="42">
+        <f t="shared" si="6"/>
+        <v>207770090</v>
+      </c>
+      <c r="G27" s="42">
+        <f t="shared" si="6"/>
+        <v>112032432</v>
+      </c>
+      <c r="H27" s="42">
+        <f t="shared" si="6"/>
+        <v>26550781</v>
+      </c>
+      <c r="I27" s="42">
+        <f t="shared" si="6"/>
+        <v>1266465</v>
+      </c>
+      <c r="J27" s="39"/>
+      <c r="K27" s="57">
+        <f>SUM(B27:J27)</f>
+        <v>1383234661</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="41" t="s">
+        <v>90</v>
+      </c>
+      <c r="B28" s="40">
+        <v>1246</v>
+      </c>
+      <c r="C28" s="40">
+        <v>2369</v>
+      </c>
+      <c r="D28" s="40">
+        <v>2518</v>
+      </c>
+      <c r="E28" s="40">
+        <v>2321</v>
+      </c>
+      <c r="F28" s="40">
+        <v>1930</v>
+      </c>
+      <c r="G28" s="40">
+        <v>1820</v>
+      </c>
+      <c r="H28" s="41">
+        <v>903</v>
+      </c>
+      <c r="I28" s="41">
+        <v>269</v>
+      </c>
+      <c r="J28" s="41">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="37"/>
+      <c r="B29" s="43">
+        <v>93151</v>
+      </c>
+      <c r="C29" s="43">
+        <v>89757</v>
+      </c>
+      <c r="D29" s="43">
+        <v>94553</v>
+      </c>
+      <c r="E29" s="43">
+        <v>104728</v>
+      </c>
+      <c r="F29" s="43">
+        <v>119106</v>
+      </c>
+      <c r="G29" s="43">
+        <v>116131</v>
+      </c>
+      <c r="H29" s="43">
+        <v>104233</v>
+      </c>
+      <c r="I29" s="43">
+        <v>94529</v>
+      </c>
+      <c r="J29" s="42">
+        <v>86698</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="37"/>
+      <c r="B30" s="42">
+        <f t="shared" ref="B30:J30" si="7">B28*B29</f>
+        <v>116066146</v>
+      </c>
+      <c r="C30" s="42">
+        <f t="shared" si="7"/>
+        <v>212634333</v>
+      </c>
+      <c r="D30" s="42">
+        <f t="shared" si="7"/>
+        <v>238084454</v>
+      </c>
+      <c r="E30" s="42">
+        <f t="shared" si="7"/>
+        <v>243073688</v>
+      </c>
+      <c r="F30" s="42">
+        <f t="shared" si="7"/>
+        <v>229874580</v>
+      </c>
+      <c r="G30" s="42">
+        <f t="shared" si="7"/>
+        <v>211358420</v>
+      </c>
+      <c r="H30" s="42">
+        <f t="shared" si="7"/>
+        <v>94122399</v>
+      </c>
+      <c r="I30" s="42">
+        <f t="shared" si="7"/>
+        <v>25428301</v>
+      </c>
+      <c r="J30" s="42">
+        <f t="shared" si="7"/>
+        <v>260094</v>
+      </c>
+      <c r="K30" s="57">
+        <f>SUM(B30:J30)</f>
+        <v>1370902415</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="B31" s="41">
+        <v>815</v>
+      </c>
+      <c r="C31" s="40">
+        <v>1571</v>
+      </c>
+      <c r="D31" s="40">
+        <v>1710</v>
+      </c>
+      <c r="E31" s="40">
+        <v>1396</v>
+      </c>
+      <c r="F31" s="40">
+        <v>1096</v>
+      </c>
+      <c r="G31" s="40">
+        <v>1095</v>
+      </c>
+      <c r="H31" s="41">
+        <v>626</v>
+      </c>
+      <c r="I31" s="41">
+        <v>245</v>
+      </c>
+      <c r="J31" s="41">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="37"/>
+      <c r="B32" s="43">
+        <v>99546</v>
+      </c>
+      <c r="C32" s="43">
+        <v>93632</v>
+      </c>
+      <c r="D32" s="43">
+        <v>96989</v>
+      </c>
+      <c r="E32" s="43">
+        <v>105313</v>
+      </c>
+      <c r="F32" s="43">
+        <v>123261</v>
+      </c>
+      <c r="G32" s="43">
+        <v>131919</v>
+      </c>
+      <c r="H32" s="43">
+        <v>148713</v>
+      </c>
+      <c r="I32" s="43">
+        <v>115391</v>
+      </c>
+      <c r="J32" s="43">
+        <v>108176</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="37"/>
+      <c r="B33" s="42">
+        <f t="shared" ref="B33:J33" si="8">B31*B32</f>
+        <v>81129990</v>
+      </c>
+      <c r="C33" s="42">
+        <f t="shared" si="8"/>
+        <v>147095872</v>
+      </c>
+      <c r="D33" s="42">
+        <f t="shared" si="8"/>
+        <v>165851190</v>
+      </c>
+      <c r="E33" s="42">
+        <f t="shared" si="8"/>
+        <v>147016948</v>
+      </c>
+      <c r="F33" s="42">
+        <f t="shared" si="8"/>
+        <v>135094056</v>
+      </c>
+      <c r="G33" s="42">
+        <f t="shared" si="8"/>
+        <v>144451305</v>
+      </c>
+      <c r="H33" s="42">
+        <f t="shared" si="8"/>
+        <v>93094338</v>
+      </c>
+      <c r="I33" s="42">
+        <f t="shared" si="8"/>
+        <v>28270795</v>
+      </c>
+      <c r="J33" s="42">
+        <f t="shared" si="8"/>
+        <v>3028928</v>
+      </c>
+      <c r="K33" s="57">
+        <f>SUM(B33:J33)</f>
+        <v>945033422</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="41" t="s">
+        <v>92</v>
+      </c>
+      <c r="B34" s="41">
+        <v>268</v>
+      </c>
+      <c r="C34" s="41">
+        <v>610</v>
+      </c>
+      <c r="D34" s="41">
+        <v>613</v>
+      </c>
+      <c r="E34" s="41">
+        <v>480</v>
+      </c>
+      <c r="F34" s="41">
+        <v>380</v>
+      </c>
+      <c r="G34" s="41">
+        <v>351</v>
+      </c>
+      <c r="H34" s="41">
+        <v>295</v>
+      </c>
+      <c r="I34" s="41">
+        <v>224</v>
+      </c>
+      <c r="J34" s="41">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="37"/>
+      <c r="B35" s="43">
+        <v>109046</v>
+      </c>
+      <c r="C35" s="43">
+        <v>100493</v>
+      </c>
+      <c r="D35" s="43">
+        <v>111602</v>
+      </c>
+      <c r="E35" s="43">
+        <v>112632</v>
+      </c>
+      <c r="F35" s="43">
+        <v>134768</v>
+      </c>
+      <c r="G35" s="43">
+        <v>147005</v>
+      </c>
+      <c r="H35" s="43">
+        <v>167347</v>
+      </c>
+      <c r="I35" s="43">
+        <v>186061</v>
+      </c>
+      <c r="J35" s="43">
+        <v>176875</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="37"/>
+      <c r="B36" s="42">
+        <f t="shared" ref="B36:J36" si="9">B34*B35</f>
+        <v>29224328</v>
+      </c>
+      <c r="C36" s="42">
+        <f t="shared" si="9"/>
+        <v>61300730</v>
+      </c>
+      <c r="D36" s="42">
+        <f t="shared" si="9"/>
+        <v>68412026</v>
+      </c>
+      <c r="E36" s="42">
+        <f t="shared" si="9"/>
+        <v>54063360</v>
+      </c>
+      <c r="F36" s="42">
+        <f t="shared" si="9"/>
+        <v>51211840</v>
+      </c>
+      <c r="G36" s="42">
+        <f t="shared" si="9"/>
+        <v>51598755</v>
+      </c>
+      <c r="H36" s="42">
+        <f t="shared" si="9"/>
+        <v>49367365</v>
+      </c>
+      <c r="I36" s="42">
+        <f t="shared" si="9"/>
+        <v>41677664</v>
+      </c>
+      <c r="J36" s="42">
+        <f t="shared" si="9"/>
+        <v>12381250</v>
+      </c>
+      <c r="K36" s="57">
+        <f>SUM(B36:J36)</f>
+        <v>419237318</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="38" t="s">
+        <v>93</v>
+      </c>
+      <c r="B37" s="41">
+        <v>132</v>
+      </c>
+      <c r="C37" s="41">
+        <v>164</v>
+      </c>
+      <c r="D37" s="41">
+        <v>172</v>
+      </c>
+      <c r="E37" s="41">
+        <v>141</v>
+      </c>
+      <c r="F37" s="41">
+        <v>121</v>
+      </c>
+      <c r="G37" s="41">
+        <v>133</v>
+      </c>
+      <c r="H37" s="41">
+        <v>115</v>
+      </c>
+      <c r="I37" s="41">
+        <v>141</v>
+      </c>
+      <c r="J37" s="41">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="37"/>
+      <c r="B38" s="43">
+        <v>120037</v>
+      </c>
+      <c r="C38" s="43">
+        <v>120246</v>
+      </c>
+      <c r="D38" s="43">
+        <v>133740</v>
+      </c>
+      <c r="E38" s="43">
+        <v>152829</v>
+      </c>
+      <c r="F38" s="43">
+        <v>158421</v>
+      </c>
+      <c r="G38" s="43">
+        <v>182235</v>
+      </c>
+      <c r="H38" s="43">
+        <v>198905</v>
+      </c>
+      <c r="I38" s="43">
+        <v>201823</v>
+      </c>
+      <c r="J38" s="43">
+        <v>199972</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="37"/>
+      <c r="B39" s="42">
+        <f t="shared" ref="B39:J39" si="10">B37*B38</f>
+        <v>15844884</v>
+      </c>
+      <c r="C39" s="42">
+        <f t="shared" si="10"/>
+        <v>19720344</v>
+      </c>
+      <c r="D39" s="42">
+        <f t="shared" si="10"/>
+        <v>23003280</v>
+      </c>
+      <c r="E39" s="42">
+        <f t="shared" si="10"/>
+        <v>21548889</v>
+      </c>
+      <c r="F39" s="42">
+        <f t="shared" si="10"/>
+        <v>19168941</v>
+      </c>
+      <c r="G39" s="42">
+        <f t="shared" si="10"/>
+        <v>24237255</v>
+      </c>
+      <c r="H39" s="42">
+        <f t="shared" si="10"/>
+        <v>22874075</v>
+      </c>
+      <c r="I39" s="42">
+        <f t="shared" si="10"/>
+        <v>28457043</v>
+      </c>
+      <c r="J39" s="42">
+        <f t="shared" si="10"/>
+        <v>43593896</v>
+      </c>
+      <c r="K39" s="57">
+        <f>SUM(B39:J39)</f>
+        <v>218448607</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="B40" s="40">
+        <v>22401</v>
+      </c>
+      <c r="C40" s="40">
+        <v>27903</v>
+      </c>
+      <c r="D40" s="40">
+        <v>19244</v>
+      </c>
+      <c r="E40" s="40">
+        <v>11568</v>
+      </c>
+      <c r="F40" s="40">
+        <v>6739</v>
+      </c>
+      <c r="G40" s="40">
+        <v>4967</v>
+      </c>
+      <c r="H40" s="40">
+        <v>2243</v>
+      </c>
+      <c r="I40" s="41">
+        <v>894</v>
+      </c>
+      <c r="J40" s="41">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="37"/>
+      <c r="B41" s="42">
+        <v>82337</v>
+      </c>
+      <c r="C41" s="42">
+        <v>88439</v>
+      </c>
+      <c r="D41" s="42">
+        <v>93978</v>
+      </c>
+      <c r="E41" s="42">
+        <v>101272</v>
+      </c>
+      <c r="F41" s="42">
+        <v>113443</v>
+      </c>
+      <c r="G41" s="42">
+        <v>115372</v>
+      </c>
+      <c r="H41" s="42">
+        <v>127861</v>
+      </c>
+      <c r="I41" s="42">
+        <v>139933</v>
+      </c>
+      <c r="J41" s="42">
+        <v>185781</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B42" s="57"/>
+      <c r="C42" s="57"/>
+      <c r="D42" s="57"/>
+      <c r="E42" s="57"/>
+      <c r="F42" s="57"/>
+      <c r="G42" s="57"/>
+      <c r="H42" s="57"/>
+      <c r="I42" s="57"/>
+      <c r="J42" s="57"/>
+      <c r="K42" s="57">
+        <f>SUM(K9:K39)</f>
+        <v>9100878611</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B43" s="57"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="E5:F5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D79" sqref="D79"/>
+      <selection activeCell="C16" sqref="C16:E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="15"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="4"/>
+      <c r="B5" s="50" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" s="50"/>
+      <c r="D5" s="50"/>
+      <c r="E5" s="50"/>
+      <c r="F5" s="9"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="47" t="s">
+        <v>102</v>
+      </c>
+      <c r="D6" s="47" t="s">
+        <v>103</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="F6" s="35" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="34" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="25">
+        <v>1024</v>
+      </c>
+      <c r="C7" s="25"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="26">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="25">
+        <v>7321</v>
+      </c>
+      <c r="C8" s="25">
+        <v>204</v>
+      </c>
+      <c r="D8" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="26">
+        <v>7525</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="25">
+        <v>8546</v>
+      </c>
+      <c r="C9" s="25">
+        <v>2041</v>
+      </c>
+      <c r="D9" s="25">
+        <v>42</v>
+      </c>
+      <c r="E9" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="26">
+        <v>10629</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="25">
+        <v>4315</v>
+      </c>
+      <c r="C10" s="25">
+        <v>2542</v>
+      </c>
+      <c r="D10" s="25">
+        <v>183</v>
+      </c>
+      <c r="E10" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="26">
+        <v>7040</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="25">
+        <v>3409</v>
+      </c>
+      <c r="C11" s="25">
+        <v>3981</v>
+      </c>
+      <c r="D11" s="25">
+        <v>493</v>
+      </c>
+      <c r="E11" s="25">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>67</v>
+      <c r="F11" s="26">
+        <v>7885</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="25">
+        <v>2440</v>
+      </c>
+      <c r="C12" s="25">
+        <v>4933</v>
+      </c>
+      <c r="D12" s="25">
+        <v>954</v>
+      </c>
+      <c r="E12" s="25">
+        <v>45</v>
+      </c>
+      <c r="F12" s="26">
+        <v>8372</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="25">
+        <v>2286</v>
+      </c>
+      <c r="C13" s="25">
+        <v>4901</v>
+      </c>
+      <c r="D13" s="25">
+        <v>1330</v>
+      </c>
+      <c r="E13" s="25">
+        <v>82</v>
+      </c>
+      <c r="F13" s="26">
+        <v>8599</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="25">
+        <v>1997</v>
+      </c>
+      <c r="C14" s="25">
+        <v>4034</v>
+      </c>
+      <c r="D14" s="25">
+        <v>1183</v>
+      </c>
+      <c r="E14" s="25">
+        <v>93</v>
+      </c>
+      <c r="F14" s="26">
+        <v>7307</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="34" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="25">
+        <v>2902</v>
+      </c>
+      <c r="C15" s="25">
+        <v>1892</v>
+      </c>
+      <c r="D15" s="25">
+        <v>400</v>
+      </c>
+      <c r="E15" s="25">
+        <v>39</v>
+      </c>
+      <c r="F15" s="26">
+        <v>5233</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="26">
+        <v>34240</v>
+      </c>
+      <c r="C16" s="26">
+        <v>24528</v>
+      </c>
+      <c r="D16" s="26">
+        <v>4585</v>
+      </c>
+      <c r="E16" s="26">
+        <v>261</v>
+      </c>
+      <c r="F16" s="26">
+        <v>63614</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B5:E5"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E13"/>
   <sheetViews>
@@ -1055,12 +2577,12 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="22"/>
-      <c r="B3" s="49" t="s">
+      <c r="B3" s="50" t="s">
         <v>48</v>
       </c>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="49"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
     </row>
     <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="34" t="s">
@@ -1234,7 +2756,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C12"/>
   <sheetViews>
@@ -1371,7 +2893,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C12"/>
   <sheetViews>
@@ -1508,19 +3030,20 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K30"/>
+  <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView topLeftCell="C4" workbookViewId="0">
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="14.85546875" customWidth="1"/>
+    <col min="7" max="11" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1539,25 +3062,25 @@
       <c r="K1" s="38"/>
     </row>
     <row r="2" spans="1:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="51" t="s">
         <v>73</v>
       </c>
-      <c r="B2" s="51"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="52"/>
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="53"/>
       <c r="I2" s="37"/>
       <c r="J2" s="37"/>
       <c r="K2" s="37"/>
     </row>
     <row r="3" spans="1:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="53" t="s">
+      <c r="A3" s="54" t="s">
         <v>74</v>
       </c>
-      <c r="B3" s="54"/>
+      <c r="B3" s="55"/>
       <c r="C3" s="38"/>
       <c r="D3" s="38"/>
       <c r="E3" s="38"/>
@@ -1569,14 +3092,14 @@
       <c r="K3" s="38"/>
     </row>
     <row r="4" spans="1:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="50" t="s">
+      <c r="A4" s="51" t="s">
         <v>94</v>
       </c>
-      <c r="B4" s="51"/>
-      <c r="C4" s="51"/>
-      <c r="D4" s="51"/>
-      <c r="E4" s="51"/>
-      <c r="F4" s="52"/>
+      <c r="B4" s="52"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="53"/>
       <c r="G4" s="37"/>
       <c r="H4" s="37"/>
       <c r="I4" s="37"/>
@@ -1589,10 +3112,10 @@
       <c r="C5" s="38"/>
       <c r="D5" s="38"/>
       <c r="E5" s="38"/>
-      <c r="F5" s="53" t="s">
+      <c r="F5" s="54" t="s">
         <v>48</v>
       </c>
-      <c r="G5" s="54"/>
+      <c r="G5" s="55"/>
       <c r="H5" s="38"/>
       <c r="I5" s="38"/>
       <c r="J5" s="38"/>
@@ -2448,6 +3971,20 @@
       <c r="K30" s="42">
         <v>185781</v>
       </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C31" s="57"/>
+      <c r="D31" s="57"/>
+      <c r="E31" s="57"/>
+      <c r="F31" s="57"/>
+      <c r="G31" s="57"/>
+      <c r="H31" s="57"/>
+      <c r="I31" s="57"/>
+      <c r="J31" s="57"/>
+      <c r="K31" s="57"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C32" s="57"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2461,7 +3998,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K31"/>
   <sheetViews>
@@ -2481,17 +4018,17 @@
       <c r="A1" s="37" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="51" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
-      <c r="I1" s="51"/>
-      <c r="J1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
+      <c r="I1" s="52"/>
+      <c r="J1" s="53"/>
       <c r="K1" s="37"/>
     </row>
     <row r="2" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2510,26 +4047,26 @@
       <c r="K2" s="38"/>
     </row>
     <row r="3" spans="1:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="50" t="s">
+      <c r="A3" s="51" t="s">
         <v>73</v>
       </c>
-      <c r="B3" s="51"/>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="51"/>
-      <c r="H3" s="52"/>
+      <c r="B3" s="52"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
+      <c r="G3" s="52"/>
+      <c r="H3" s="53"/>
       <c r="I3" s="37"/>
       <c r="J3" s="37"/>
       <c r="K3" s="37"/>
     </row>
     <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="53" t="s">
+      <c r="A4" s="54" t="s">
         <v>74</v>
       </c>
-      <c r="B4" s="55"/>
-      <c r="C4" s="54"/>
+      <c r="B4" s="56"/>
+      <c r="C4" s="55"/>
       <c r="D4" s="38"/>
       <c r="E4" s="38"/>
       <c r="F4" s="38"/>
@@ -2540,18 +4077,18 @@
       <c r="K4" s="38"/>
     </row>
     <row r="5" spans="1:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="50" t="s">
+      <c r="A5" s="51" t="s">
         <v>95</v>
       </c>
-      <c r="B5" s="51"/>
-      <c r="C5" s="51"/>
-      <c r="D5" s="51"/>
-      <c r="E5" s="51"/>
-      <c r="F5" s="51"/>
-      <c r="G5" s="51"/>
-      <c r="H5" s="51"/>
-      <c r="I5" s="51"/>
-      <c r="J5" s="52"/>
+      <c r="B5" s="52"/>
+      <c r="C5" s="52"/>
+      <c r="D5" s="52"/>
+      <c r="E5" s="52"/>
+      <c r="F5" s="52"/>
+      <c r="G5" s="52"/>
+      <c r="H5" s="52"/>
+      <c r="I5" s="52"/>
+      <c r="J5" s="53"/>
       <c r="K5" s="37"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2560,10 +4097,10 @@
       <c r="C6" s="38"/>
       <c r="D6" s="38"/>
       <c r="E6" s="38"/>
-      <c r="F6" s="53" t="s">
+      <c r="F6" s="54" t="s">
         <v>48</v>
       </c>
-      <c r="G6" s="54"/>
+      <c r="G6" s="55"/>
       <c r="H6" s="38"/>
       <c r="I6" s="38"/>
       <c r="J6" s="38"/>
@@ -3432,7 +4969,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K32"/>
   <sheetViews>
@@ -3452,17 +4989,17 @@
       <c r="A1" s="37" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="51" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
-      <c r="I1" s="51"/>
-      <c r="J1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
+      <c r="I1" s="52"/>
+      <c r="J1" s="53"/>
       <c r="K1" s="37"/>
     </row>
     <row r="2" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3481,26 +5018,26 @@
       <c r="K2" s="38"/>
     </row>
     <row r="3" spans="1:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="50" t="s">
+      <c r="A3" s="51" t="s">
         <v>73</v>
       </c>
-      <c r="B3" s="51"/>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="51"/>
-      <c r="H3" s="52"/>
+      <c r="B3" s="52"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
+      <c r="G3" s="52"/>
+      <c r="H3" s="53"/>
       <c r="I3" s="37"/>
       <c r="J3" s="37"/>
       <c r="K3" s="37"/>
     </row>
     <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="53" t="s">
+      <c r="A4" s="54" t="s">
         <v>74</v>
       </c>
-      <c r="B4" s="55"/>
-      <c r="C4" s="54"/>
+      <c r="B4" s="56"/>
+      <c r="C4" s="55"/>
       <c r="D4" s="38"/>
       <c r="E4" s="38"/>
       <c r="F4" s="38"/>
@@ -3511,18 +5048,18 @@
       <c r="K4" s="38"/>
     </row>
     <row r="5" spans="1:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="50" t="s">
+      <c r="A5" s="51" t="s">
         <v>96</v>
       </c>
-      <c r="B5" s="51"/>
-      <c r="C5" s="51"/>
-      <c r="D5" s="51"/>
-      <c r="E5" s="51"/>
-      <c r="F5" s="51"/>
-      <c r="G5" s="51"/>
-      <c r="H5" s="51"/>
-      <c r="I5" s="51"/>
-      <c r="J5" s="52"/>
+      <c r="B5" s="52"/>
+      <c r="C5" s="52"/>
+      <c r="D5" s="52"/>
+      <c r="E5" s="52"/>
+      <c r="F5" s="52"/>
+      <c r="G5" s="52"/>
+      <c r="H5" s="52"/>
+      <c r="I5" s="52"/>
+      <c r="J5" s="53"/>
       <c r="K5" s="37"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3546,10 +5083,10 @@
       <c r="C7" s="37"/>
       <c r="D7" s="37"/>
       <c r="E7" s="37"/>
-      <c r="F7" s="50" t="s">
+      <c r="F7" s="51" t="s">
         <v>48</v>
       </c>
-      <c r="G7" s="52"/>
+      <c r="G7" s="53"/>
       <c r="H7" s="37"/>
       <c r="I7" s="37"/>
       <c r="J7" s="37"/>
@@ -4418,7 +5955,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K31"/>
   <sheetViews>
@@ -4440,17 +5977,17 @@
       <c r="A1" s="37" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="51" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
-      <c r="I1" s="51"/>
-      <c r="J1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
+      <c r="I1" s="52"/>
+      <c r="J1" s="53"/>
       <c r="K1" s="37"/>
     </row>
     <row r="2" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4469,25 +6006,25 @@
       <c r="K2" s="38"/>
     </row>
     <row r="3" spans="1:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="50" t="s">
+      <c r="A3" s="51" t="s">
         <v>73</v>
       </c>
-      <c r="B3" s="51"/>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="51"/>
-      <c r="H3" s="52"/>
+      <c r="B3" s="52"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
+      <c r="G3" s="52"/>
+      <c r="H3" s="53"/>
       <c r="I3" s="37"/>
       <c r="J3" s="37"/>
       <c r="K3" s="37"/>
     </row>
     <row r="4" spans="1:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="53" t="s">
+      <c r="A4" s="54" t="s">
         <v>74</v>
       </c>
-      <c r="B4" s="54"/>
+      <c r="B4" s="55"/>
       <c r="C4" s="38"/>
       <c r="D4" s="38"/>
       <c r="E4" s="38"/>
@@ -4499,10 +6036,10 @@
       <c r="K4" s="38"/>
     </row>
     <row r="5" spans="1:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="50" t="s">
+      <c r="A5" s="51" t="s">
         <v>98</v>
       </c>
-      <c r="B5" s="52"/>
+      <c r="B5" s="53"/>
       <c r="C5" s="37"/>
       <c r="D5" s="37"/>
       <c r="E5" s="37"/>
@@ -4519,10 +6056,10 @@
       <c r="C6" s="38"/>
       <c r="D6" s="38"/>
       <c r="E6" s="38"/>
-      <c r="F6" s="53" t="s">
+      <c r="F6" s="54" t="s">
         <v>48</v>
       </c>
-      <c r="G6" s="54"/>
+      <c r="G6" s="55"/>
       <c r="H6" s="38"/>
       <c r="I6" s="38"/>
       <c r="J6" s="38"/>
@@ -5392,6 +6929,47 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:A9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D79" sqref="D79"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J122"/>
   <sheetViews>
@@ -5771,12 +7349,12 @@
     </row>
     <row r="35" spans="1:6" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
-      <c r="B35" s="49" t="s">
+      <c r="B35" s="50" t="s">
         <v>48</v>
       </c>
-      <c r="C35" s="49"/>
-      <c r="D35" s="49"/>
-      <c r="E35" s="49"/>
+      <c r="C35" s="50"/>
+      <c r="D35" s="50"/>
+      <c r="E35" s="50"/>
     </row>
     <row r="36" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
@@ -6008,12 +7586,12 @@
     </row>
     <row r="51" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="22"/>
-      <c r="B51" s="49" t="s">
+      <c r="B51" s="50" t="s">
         <v>48</v>
       </c>
-      <c r="C51" s="49"/>
-      <c r="D51" s="49"/>
-      <c r="E51" s="49"/>
+      <c r="C51" s="50"/>
+      <c r="D51" s="50"/>
+      <c r="E51" s="50"/>
     </row>
     <row r="52" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
@@ -6203,12 +7781,12 @@
     </row>
     <row r="68" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="22"/>
-      <c r="B68" s="49" t="s">
+      <c r="B68" s="50" t="s">
         <v>48</v>
       </c>
-      <c r="C68" s="49"/>
-      <c r="D68" s="49"/>
-      <c r="E68" s="49"/>
+      <c r="C68" s="50"/>
+      <c r="D68" s="50"/>
+      <c r="E68" s="50"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
@@ -6317,12 +7895,12 @@
     </row>
     <row r="78" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="4"/>
-      <c r="B78" s="49" t="s">
+      <c r="B78" s="50" t="s">
         <v>48</v>
       </c>
-      <c r="C78" s="49"/>
-      <c r="D78" s="49"/>
-      <c r="E78" s="49"/>
+      <c r="C78" s="50"/>
+      <c r="D78" s="50"/>
+      <c r="E78" s="50"/>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="17" t="s">
@@ -6574,7 +8152,7 @@
       <c r="J101" s="12"/>
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A102" s="48" t="s">
+      <c r="A102" s="49" t="s">
         <v>65</v>
       </c>
       <c r="B102" s="6" t="s">
@@ -6600,7 +8178,7 @@
       <c r="J102" s="12"/>
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A103" s="48"/>
+      <c r="A103" s="49"/>
       <c r="B103" s="6" t="s">
         <v>12</v>
       </c>
@@ -6624,7 +8202,7 @@
       <c r="J103" s="12"/>
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A104" s="48" t="s">
+      <c r="A104" s="49" t="s">
         <v>13</v>
       </c>
       <c r="B104" s="6" t="s">
@@ -6650,7 +8228,7 @@
       <c r="J104" s="12"/>
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A105" s="48"/>
+      <c r="A105" s="49"/>
       <c r="B105" s="6" t="s">
         <v>12</v>
       </c>
@@ -6674,7 +8252,7 @@
       <c r="J105" s="12"/>
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A106" s="48" t="s">
+      <c r="A106" s="49" t="s">
         <v>14</v>
       </c>
       <c r="B106" s="6" t="s">
@@ -6700,7 +8278,7 @@
       <c r="J106" s="12"/>
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A107" s="48"/>
+      <c r="A107" s="49"/>
       <c r="B107" s="6" t="s">
         <v>12</v>
       </c>
@@ -6973,7 +8551,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -7030,7 +8608,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
@@ -7129,7 +8707,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G8"/>
   <sheetViews>
@@ -7319,7 +8897,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
@@ -7423,7 +9001,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
@@ -7451,12 +9029,12 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
-      <c r="B3" s="49" t="s">
+      <c r="B3" s="50" t="s">
         <v>48</v>
       </c>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="49"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="35" t="s">
@@ -7566,7 +9144,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
@@ -7603,12 +9181,12 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="22"/>
-      <c r="B4" s="49" t="s">
+      <c r="B4" s="50" t="s">
         <v>48</v>
       </c>
-      <c r="C4" s="49"/>
-      <c r="D4" s="49"/>
-      <c r="E4" s="49"/>
+      <c r="C4" s="50"/>
+      <c r="D4" s="50"/>
+      <c r="E4" s="50"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="34" t="s">
@@ -7716,282 +9294,4 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F16"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16:E16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="15"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="49" t="s">
-        <v>48</v>
-      </c>
-      <c r="C5" s="49"/>
-      <c r="D5" s="49"/>
-      <c r="E5" s="49"/>
-      <c r="F5" s="9"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="34" t="s">
-        <v>44</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C6" s="47" t="s">
-        <v>102</v>
-      </c>
-      <c r="D6" s="47" t="s">
-        <v>103</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="F6" s="35" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="34" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="25">
-        <v>1024</v>
-      </c>
-      <c r="C7" s="25"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="26">
-        <v>1024</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="34" t="s">
-        <v>37</v>
-      </c>
-      <c r="B8" s="25">
-        <v>7321</v>
-      </c>
-      <c r="C8" s="25">
-        <v>204</v>
-      </c>
-      <c r="D8" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="26">
-        <v>7525</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="34" t="s">
-        <v>38</v>
-      </c>
-      <c r="B9" s="25">
-        <v>8546</v>
-      </c>
-      <c r="C9" s="25">
-        <v>2041</v>
-      </c>
-      <c r="D9" s="25">
-        <v>42</v>
-      </c>
-      <c r="E9" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" s="26">
-        <v>10629</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="34" t="s">
-        <v>39</v>
-      </c>
-      <c r="B10" s="25">
-        <v>4315</v>
-      </c>
-      <c r="C10" s="25">
-        <v>2542</v>
-      </c>
-      <c r="D10" s="25">
-        <v>183</v>
-      </c>
-      <c r="E10" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" s="26">
-        <v>7040</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="B11" s="25">
-        <v>3409</v>
-      </c>
-      <c r="C11" s="25">
-        <v>3981</v>
-      </c>
-      <c r="D11" s="25">
-        <v>493</v>
-      </c>
-      <c r="E11" s="25">
-        <v>2</v>
-      </c>
-      <c r="F11" s="26">
-        <v>7885</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="34" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" s="25">
-        <v>2440</v>
-      </c>
-      <c r="C12" s="25">
-        <v>4933</v>
-      </c>
-      <c r="D12" s="25">
-        <v>954</v>
-      </c>
-      <c r="E12" s="25">
-        <v>45</v>
-      </c>
-      <c r="F12" s="26">
-        <v>8372</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="25">
-        <v>2286</v>
-      </c>
-      <c r="C13" s="25">
-        <v>4901</v>
-      </c>
-      <c r="D13" s="25">
-        <v>1330</v>
-      </c>
-      <c r="E13" s="25">
-        <v>82</v>
-      </c>
-      <c r="F13" s="26">
-        <v>8599</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="34" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" s="25">
-        <v>1997</v>
-      </c>
-      <c r="C14" s="25">
-        <v>4034</v>
-      </c>
-      <c r="D14" s="25">
-        <v>1183</v>
-      </c>
-      <c r="E14" s="25">
-        <v>93</v>
-      </c>
-      <c r="F14" s="26">
-        <v>7307</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="34" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15" s="25">
-        <v>2902</v>
-      </c>
-      <c r="C15" s="25">
-        <v>1892</v>
-      </c>
-      <c r="D15" s="25">
-        <v>400</v>
-      </c>
-      <c r="E15" s="25">
-        <v>39</v>
-      </c>
-      <c r="F15" s="26">
-        <v>5233</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="B16" s="26">
-        <v>34240</v>
-      </c>
-      <c r="C16" s="26">
-        <v>24528</v>
-      </c>
-      <c r="D16" s="26">
-        <v>4585</v>
-      </c>
-      <c r="E16" s="26">
-        <v>261</v>
-      </c>
-      <c r="F16" s="26">
-        <v>63614</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B5:E5"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
add imputation for actives.
</commit_message>
<xml_diff>
--- a/Data/UCRP-MembersData-2015.xlsx
+++ b/Data/UCRP-MembersData-2015.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="24900" firstSheet="9" activeTab="12"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="24900" firstSheet="12" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="Active_t76 (2)" sheetId="21" r:id="rId1"/>
@@ -532,7 +532,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -689,6 +689,27 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="6" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2900,7 +2921,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
@@ -3035,959 +3056,1032 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K32"/>
+  <dimension ref="A1:L34"/>
   <sheetViews>
-    <sheetView topLeftCell="C4" workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="14.85546875" customWidth="1"/>
-    <col min="7" max="11" width="13.7109375" customWidth="1"/>
+    <col min="1" max="1" width="8.42578125" style="60" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" style="60" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="14.85546875" style="60" customWidth="1"/>
+    <col min="7" max="11" width="13.7109375" style="60" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="60"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="38" t="s">
+    <row r="1" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="58" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
-      <c r="K1" s="38"/>
-    </row>
-    <row r="2" spans="1:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="50" t="s">
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="58"/>
+      <c r="J1" s="58"/>
+      <c r="K1" s="58"/>
+      <c r="L1" s="59"/>
+    </row>
+    <row r="2" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="61" t="s">
         <v>73</v>
       </c>
-      <c r="B2" s="51"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
-    </row>
-    <row r="3" spans="1:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="53" t="s">
+      <c r="B2" s="61"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="58"/>
+      <c r="J2" s="58"/>
+      <c r="K2" s="58"/>
+      <c r="L2" s="59"/>
+    </row>
+    <row r="3" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="61" t="s">
         <v>74</v>
       </c>
-      <c r="B3" s="54"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
-      <c r="K3" s="38"/>
-    </row>
-    <row r="4" spans="1:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="50" t="s">
+      <c r="B3" s="61"/>
+      <c r="C3" s="58"/>
+      <c r="D3" s="58"/>
+      <c r="E3" s="58"/>
+      <c r="F3" s="58"/>
+      <c r="G3" s="58"/>
+      <c r="H3" s="58"/>
+      <c r="I3" s="58"/>
+      <c r="J3" s="58"/>
+      <c r="K3" s="58"/>
+      <c r="L3" s="59"/>
+    </row>
+    <row r="4" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="61" t="s">
         <v>94</v>
       </c>
-      <c r="B4" s="51"/>
-      <c r="C4" s="51"/>
-      <c r="D4" s="51"/>
-      <c r="E4" s="51"/>
-      <c r="F4" s="52"/>
-      <c r="G4" s="37"/>
-      <c r="H4" s="37"/>
-      <c r="I4" s="37"/>
-      <c r="J4" s="37"/>
-      <c r="K4" s="37"/>
-    </row>
-    <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="38"/>
-      <c r="B5" s="38"/>
-      <c r="C5" s="38"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="53" t="s">
+      <c r="B4" s="61"/>
+      <c r="C4" s="61"/>
+      <c r="D4" s="61"/>
+      <c r="E4" s="61"/>
+      <c r="F4" s="61"/>
+      <c r="G4" s="58"/>
+      <c r="H4" s="58"/>
+      <c r="I4" s="58"/>
+      <c r="J4" s="58"/>
+      <c r="K4" s="58"/>
+      <c r="L4" s="59"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="58"/>
+      <c r="B5" s="58"/>
+      <c r="C5" s="58"/>
+      <c r="D5" s="58"/>
+      <c r="E5" s="58"/>
+      <c r="F5" s="61" t="s">
         <v>48</v>
       </c>
-      <c r="G5" s="54"/>
-      <c r="H5" s="38"/>
-      <c r="I5" s="38"/>
-      <c r="J5" s="38"/>
-      <c r="K5" s="38"/>
-    </row>
-    <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="37" t="s">
+      <c r="G5" s="61"/>
+      <c r="H5" s="58"/>
+      <c r="I5" s="58"/>
+      <c r="J5" s="58"/>
+      <c r="K5" s="58"/>
+      <c r="L5" s="59"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="58" t="s">
         <v>44</v>
       </c>
-      <c r="B6" s="37" t="s">
+      <c r="B6" s="58" t="s">
         <v>42</v>
       </c>
-      <c r="C6" s="39" t="s">
+      <c r="C6" s="62" t="s">
         <v>75</v>
       </c>
-      <c r="D6" s="45" t="s">
+      <c r="D6" s="63" t="s">
         <v>99</v>
       </c>
-      <c r="E6" s="45" t="s">
+      <c r="E6" s="63" t="s">
         <v>100</v>
       </c>
-      <c r="F6" s="39" t="s">
+      <c r="F6" s="62" t="s">
         <v>76</v>
       </c>
-      <c r="G6" s="39" t="s">
+      <c r="G6" s="62" t="s">
         <v>77</v>
       </c>
-      <c r="H6" s="39" t="s">
+      <c r="H6" s="62" t="s">
         <v>78</v>
       </c>
-      <c r="I6" s="39" t="s">
+      <c r="I6" s="62" t="s">
         <v>79</v>
       </c>
-      <c r="J6" s="39" t="s">
+      <c r="J6" s="62" t="s">
         <v>80</v>
       </c>
-      <c r="K6" s="37" t="s">
+      <c r="K6" s="58" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="38" t="s">
+      <c r="L6" s="59"/>
+    </row>
+    <row r="7" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="58" t="s">
         <v>82</v>
       </c>
-      <c r="B7" s="41">
+      <c r="B7" s="62">
         <v>466</v>
       </c>
-      <c r="C7" s="41">
+      <c r="C7" s="62">
         <v>450</v>
       </c>
-      <c r="D7" s="41">
+      <c r="D7" s="62">
         <v>16</v>
       </c>
-      <c r="E7" s="41" t="s">
-        <v>83</v>
-      </c>
-      <c r="F7" s="41" t="s">
-        <v>83</v>
-      </c>
-      <c r="G7" s="41" t="s">
-        <v>83</v>
-      </c>
-      <c r="H7" s="41" t="s">
-        <v>83</v>
-      </c>
-      <c r="I7" s="41" t="s">
-        <v>83</v>
-      </c>
-      <c r="J7" s="41" t="s">
-        <v>83</v>
-      </c>
-      <c r="K7" s="41" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="37"/>
-      <c r="B8" s="42">
+      <c r="E7" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="F7" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="G7" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="H7" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="I7" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="J7" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="K7" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="L7" s="59"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="58"/>
+      <c r="B8" s="64">
         <v>48912</v>
       </c>
-      <c r="C8" s="42">
+      <c r="C8" s="64">
         <v>49125</v>
       </c>
-      <c r="D8" s="42">
+      <c r="D8" s="64">
         <v>42899</v>
       </c>
-      <c r="E8" s="39" t="s">
-        <v>83</v>
-      </c>
-      <c r="F8" s="39" t="s">
-        <v>83</v>
-      </c>
-      <c r="G8" s="39" t="s">
-        <v>83</v>
-      </c>
-      <c r="H8" s="39" t="s">
-        <v>83</v>
-      </c>
-      <c r="I8" s="39" t="s">
-        <v>83</v>
-      </c>
-      <c r="J8" s="39" t="s">
-        <v>83</v>
-      </c>
-      <c r="K8" s="39" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="41" t="s">
+      <c r="E8" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="F8" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="G8" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="H8" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="I8" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="J8" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="K8" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="L8" s="59"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="62" t="s">
         <v>84</v>
       </c>
-      <c r="B9" s="40">
+      <c r="B9" s="65">
         <v>5222</v>
       </c>
-      <c r="C9" s="40">
+      <c r="C9" s="65">
         <v>4091</v>
       </c>
-      <c r="D9" s="40">
+      <c r="D9" s="65">
         <v>1113</v>
       </c>
-      <c r="E9" s="41">
+      <c r="E9" s="62">
         <v>18</v>
       </c>
-      <c r="F9" s="41" t="s">
-        <v>83</v>
-      </c>
-      <c r="G9" s="41" t="s">
-        <v>83</v>
-      </c>
-      <c r="H9" s="41" t="s">
-        <v>83</v>
-      </c>
-      <c r="I9" s="41" t="s">
-        <v>83</v>
-      </c>
-      <c r="J9" s="41" t="s">
-        <v>83</v>
-      </c>
-      <c r="K9" s="41" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="37"/>
-      <c r="B10" s="43">
+      <c r="F9" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="G9" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="H9" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="I9" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="J9" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="K9" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="L9" s="59"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="58"/>
+      <c r="B10" s="65">
         <v>62098</v>
       </c>
-      <c r="C10" s="43">
+      <c r="C10" s="65">
         <v>62836</v>
       </c>
-      <c r="D10" s="43">
+      <c r="D10" s="65">
         <v>59637</v>
       </c>
-      <c r="E10" s="42">
+      <c r="E10" s="64">
         <v>46481</v>
       </c>
-      <c r="F10" s="39" t="s">
-        <v>83</v>
-      </c>
-      <c r="G10" s="39" t="s">
-        <v>83</v>
-      </c>
-      <c r="H10" s="39" t="s">
-        <v>83</v>
-      </c>
-      <c r="I10" s="39" t="s">
-        <v>83</v>
-      </c>
-      <c r="J10" s="39" t="s">
-        <v>83</v>
-      </c>
-      <c r="K10" s="39" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="41" t="s">
+      <c r="F10" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="G10" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="H10" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="I10" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="J10" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="K10" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="L10" s="59"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="62" t="s">
         <v>85</v>
       </c>
-      <c r="B11" s="40">
+      <c r="B11" s="65">
         <v>10004</v>
       </c>
-      <c r="C11" s="40">
+      <c r="C11" s="65">
         <v>4579</v>
       </c>
-      <c r="D11" s="40">
+      <c r="D11" s="65">
         <v>4661</v>
       </c>
-      <c r="E11" s="41">
+      <c r="E11" s="62">
         <v>744</v>
       </c>
-      <c r="F11" s="41">
+      <c r="F11" s="62">
         <v>20</v>
       </c>
-      <c r="G11" s="41" t="s">
-        <v>83</v>
-      </c>
-      <c r="H11" s="41" t="s">
-        <v>83</v>
-      </c>
-      <c r="I11" s="41" t="s">
-        <v>83</v>
-      </c>
-      <c r="J11" s="41" t="s">
-        <v>83</v>
-      </c>
-      <c r="K11" s="41" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="37"/>
-      <c r="B12" s="43">
+      <c r="G11" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="H11" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="I11" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="J11" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="K11" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="L11" s="59"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="58"/>
+      <c r="B12" s="65">
         <v>76044</v>
       </c>
-      <c r="C12" s="43">
+      <c r="C12" s="65">
         <v>77686</v>
       </c>
-      <c r="D12" s="43">
+      <c r="D12" s="65">
         <v>75964</v>
       </c>
-      <c r="E12" s="43">
+      <c r="E12" s="65">
         <v>66937</v>
       </c>
-      <c r="F12" s="42">
+      <c r="F12" s="64">
         <v>57202</v>
       </c>
-      <c r="G12" s="39" t="s">
-        <v>83</v>
-      </c>
-      <c r="H12" s="39" t="s">
-        <v>83</v>
-      </c>
-      <c r="I12" s="39" t="s">
-        <v>83</v>
-      </c>
-      <c r="J12" s="39" t="s">
-        <v>83</v>
-      </c>
-      <c r="K12" s="39" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="41" t="s">
+      <c r="G12" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="H12" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="I12" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="J12" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="K12" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="L12" s="59"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="62" t="s">
         <v>86</v>
       </c>
-      <c r="B13" s="40">
+      <c r="B13" s="65">
         <v>12494</v>
       </c>
-      <c r="C13" s="40">
+      <c r="C13" s="65">
         <v>4218</v>
       </c>
-      <c r="D13" s="40">
+      <c r="D13" s="65">
         <v>5198</v>
       </c>
-      <c r="E13" s="40">
+      <c r="E13" s="65">
         <v>2558</v>
       </c>
-      <c r="F13" s="41">
+      <c r="F13" s="62">
         <v>514</v>
       </c>
-      <c r="G13" s="41">
+      <c r="G13" s="62">
         <v>6</v>
       </c>
-      <c r="H13" s="41" t="s">
-        <v>83</v>
-      </c>
-      <c r="I13" s="41" t="s">
-        <v>83</v>
-      </c>
-      <c r="J13" s="41" t="s">
-        <v>83</v>
-      </c>
-      <c r="K13" s="41" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="37"/>
-      <c r="B14" s="43">
+      <c r="H13" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="I13" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="J13" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="K13" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="L13" s="59"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="58"/>
+      <c r="B14" s="65">
         <v>87126</v>
       </c>
-      <c r="C14" s="43">
+      <c r="C14" s="65">
         <v>88621</v>
       </c>
-      <c r="D14" s="43">
+      <c r="D14" s="65">
         <v>90614</v>
       </c>
-      <c r="E14" s="43">
+      <c r="E14" s="65">
         <v>80010</v>
       </c>
-      <c r="F14" s="43">
+      <c r="F14" s="65">
         <v>75111</v>
       </c>
-      <c r="G14" s="42">
+      <c r="G14" s="64">
         <v>77949</v>
       </c>
-      <c r="H14" s="39" t="s">
-        <v>83</v>
-      </c>
-      <c r="I14" s="39" t="s">
-        <v>83</v>
-      </c>
-      <c r="J14" s="39" t="s">
-        <v>83</v>
-      </c>
-      <c r="K14" s="39" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="41" t="s">
+      <c r="H14" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="I14" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="J14" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="K14" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="L14" s="59"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="62" t="s">
         <v>87</v>
       </c>
-      <c r="B15" s="40">
+      <c r="B15" s="65">
         <v>13609</v>
       </c>
-      <c r="C15" s="40">
+      <c r="C15" s="65">
         <v>2898</v>
       </c>
-      <c r="D15" s="40">
+      <c r="D15" s="65">
         <v>5157</v>
       </c>
-      <c r="E15" s="40">
+      <c r="E15" s="65">
         <v>3656</v>
       </c>
-      <c r="F15" s="40">
+      <c r="F15" s="65">
         <v>1582</v>
       </c>
-      <c r="G15" s="41">
+      <c r="G15" s="62">
         <v>305</v>
       </c>
-      <c r="H15" s="41">
+      <c r="H15" s="62">
         <v>11</v>
       </c>
-      <c r="I15" s="41" t="s">
-        <v>83</v>
-      </c>
-      <c r="J15" s="41" t="s">
-        <v>83</v>
-      </c>
-      <c r="K15" s="41" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="37"/>
-      <c r="B16" s="43">
+      <c r="I15" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="J15" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="K15" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="L15" s="59"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="58"/>
+      <c r="B16" s="65">
         <v>93061</v>
       </c>
-      <c r="C16" s="43">
+      <c r="C16" s="65">
         <v>89793</v>
       </c>
-      <c r="D16" s="43">
+      <c r="D16" s="65">
         <v>96293</v>
       </c>
-      <c r="E16" s="43">
+      <c r="E16" s="65">
         <v>95348</v>
       </c>
-      <c r="F16" s="43">
+      <c r="F16" s="65">
         <v>85513</v>
       </c>
-      <c r="G16" s="43">
+      <c r="G16" s="65">
         <v>81725</v>
       </c>
-      <c r="H16" s="42">
+      <c r="H16" s="64">
         <v>78205</v>
       </c>
-      <c r="I16" s="39" t="s">
-        <v>83</v>
-      </c>
-      <c r="J16" s="39" t="s">
-        <v>83</v>
-      </c>
-      <c r="K16" s="39" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="41" t="s">
+      <c r="I16" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="J16" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="K16" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="L16" s="59"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="62" t="s">
         <v>88</v>
       </c>
-      <c r="B17" s="40">
+      <c r="B17" s="65">
         <v>13645</v>
       </c>
-      <c r="C17" s="40">
+      <c r="C17" s="65">
         <v>2059</v>
       </c>
-      <c r="D17" s="40">
+      <c r="D17" s="65">
         <v>3911</v>
       </c>
-      <c r="E17" s="40">
+      <c r="E17" s="65">
         <v>3872</v>
       </c>
-      <c r="F17" s="40">
+      <c r="F17" s="65">
         <v>2416</v>
       </c>
-      <c r="G17" s="40">
+      <c r="G17" s="65">
         <v>1031</v>
       </c>
-      <c r="H17" s="41">
+      <c r="H17" s="62">
         <v>345</v>
       </c>
-      <c r="I17" s="41">
+      <c r="I17" s="62">
         <v>11</v>
       </c>
-      <c r="J17" s="41" t="s">
-        <v>83</v>
-      </c>
-      <c r="K17" s="41" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="37"/>
-      <c r="B18" s="43">
+      <c r="J17" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="K17" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="L17" s="59"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="58"/>
+      <c r="B18" s="65">
         <v>95361</v>
       </c>
-      <c r="C18" s="43">
+      <c r="C18" s="65">
         <v>88555</v>
       </c>
-      <c r="D18" s="43">
+      <c r="D18" s="65">
         <v>92609</v>
       </c>
-      <c r="E18" s="43">
+      <c r="E18" s="65">
         <v>99988</v>
       </c>
-      <c r="F18" s="43">
+      <c r="F18" s="65">
         <v>101093</v>
       </c>
-      <c r="G18" s="43">
+      <c r="G18" s="65">
         <v>93091</v>
       </c>
-      <c r="H18" s="43">
+      <c r="H18" s="65">
         <v>82653</v>
       </c>
-      <c r="I18" s="42">
+      <c r="I18" s="64">
         <v>71252</v>
       </c>
-      <c r="J18" s="39" t="s">
-        <v>83</v>
-      </c>
-      <c r="K18" s="39" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="41" t="s">
+      <c r="J18" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="K18" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="L18" s="59"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="62" t="s">
         <v>89</v>
       </c>
-      <c r="B19" s="40">
+      <c r="B19" s="65">
         <v>14249</v>
       </c>
-      <c r="C19" s="40">
+      <c r="C19" s="65">
         <v>1645</v>
       </c>
-      <c r="D19" s="40">
+      <c r="D19" s="65">
         <v>3133</v>
       </c>
-      <c r="E19" s="40">
+      <c r="E19" s="65">
         <v>3383</v>
       </c>
-      <c r="F19" s="40">
+      <c r="F19" s="65">
         <v>2698</v>
       </c>
-      <c r="G19" s="40">
+      <c r="G19" s="65">
         <v>1870</v>
       </c>
-      <c r="H19" s="40">
+      <c r="H19" s="65">
         <v>1212</v>
       </c>
-      <c r="I19" s="41">
+      <c r="I19" s="62">
         <v>293</v>
       </c>
-      <c r="J19" s="41">
+      <c r="J19" s="62">
         <v>15</v>
       </c>
-      <c r="K19" s="41" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="37"/>
-      <c r="B20" s="43">
+      <c r="K19" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="L19" s="59"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="58"/>
+      <c r="B20" s="65">
         <v>97076</v>
       </c>
-      <c r="C20" s="43">
+      <c r="C20" s="65">
         <v>91738</v>
       </c>
-      <c r="D20" s="43">
+      <c r="D20" s="65">
         <v>88111</v>
       </c>
-      <c r="E20" s="43">
+      <c r="E20" s="65">
         <v>95216</v>
       </c>
-      <c r="F20" s="43">
+      <c r="F20" s="65">
         <v>106204</v>
       </c>
-      <c r="G20" s="43">
+      <c r="G20" s="65">
         <v>111107</v>
       </c>
-      <c r="H20" s="43">
+      <c r="H20" s="65">
         <v>92436</v>
       </c>
-      <c r="I20" s="43">
+      <c r="I20" s="65">
         <v>90617</v>
       </c>
-      <c r="J20" s="42">
+      <c r="J20" s="64">
         <v>84431</v>
       </c>
-      <c r="K20" s="39" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="41" t="s">
+      <c r="K20" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="L20" s="59"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="62" t="s">
         <v>90</v>
       </c>
-      <c r="B21" s="40">
+      <c r="B21" s="65">
         <v>13379</v>
       </c>
-      <c r="C21" s="40">
+      <c r="C21" s="65">
         <v>1246</v>
       </c>
-      <c r="D21" s="40">
+      <c r="D21" s="65">
         <v>2369</v>
       </c>
-      <c r="E21" s="40">
+      <c r="E21" s="65">
         <v>2518</v>
       </c>
-      <c r="F21" s="40">
+      <c r="F21" s="65">
         <v>2321</v>
       </c>
-      <c r="G21" s="40">
+      <c r="G21" s="65">
         <v>1930</v>
       </c>
-      <c r="H21" s="40">
+      <c r="H21" s="65">
         <v>1820</v>
       </c>
-      <c r="I21" s="41">
+      <c r="I21" s="62">
         <v>903</v>
       </c>
-      <c r="J21" s="41">
+      <c r="J21" s="62">
         <v>269</v>
       </c>
-      <c r="K21" s="41">
+      <c r="K21" s="62">
         <v>3</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="37"/>
-      <c r="B22" s="43">
+      <c r="L21" s="59"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="58"/>
+      <c r="B22" s="65">
         <v>102467</v>
       </c>
-      <c r="C22" s="43">
+      <c r="C22" s="65">
         <v>93151</v>
       </c>
-      <c r="D22" s="43">
+      <c r="D22" s="65">
         <v>89757</v>
       </c>
-      <c r="E22" s="43">
+      <c r="E22" s="65">
         <v>94553</v>
       </c>
-      <c r="F22" s="43">
+      <c r="F22" s="65">
         <v>104728</v>
       </c>
-      <c r="G22" s="43">
+      <c r="G22" s="65">
         <v>119106</v>
       </c>
-      <c r="H22" s="43">
+      <c r="H22" s="65">
         <v>116131</v>
       </c>
-      <c r="I22" s="43">
+      <c r="I22" s="65">
         <v>104233</v>
       </c>
-      <c r="J22" s="43">
+      <c r="J22" s="65">
         <v>94529</v>
       </c>
-      <c r="K22" s="42">
+      <c r="K22" s="64">
         <v>86698</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="41" t="s">
+      <c r="L22" s="59"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="62" t="s">
         <v>91</v>
       </c>
-      <c r="B23" s="40">
+      <c r="B23" s="65">
         <v>8582</v>
       </c>
-      <c r="C23" s="41">
+      <c r="C23" s="62">
         <v>815</v>
       </c>
-      <c r="D23" s="40">
+      <c r="D23" s="65">
         <v>1571</v>
       </c>
-      <c r="E23" s="40">
+      <c r="E23" s="65">
         <v>1710</v>
       </c>
-      <c r="F23" s="40">
+      <c r="F23" s="65">
         <v>1396</v>
       </c>
-      <c r="G23" s="40">
+      <c r="G23" s="65">
         <v>1096</v>
       </c>
-      <c r="H23" s="40">
+      <c r="H23" s="65">
         <v>1095</v>
       </c>
-      <c r="I23" s="41">
+      <c r="I23" s="62">
         <v>626</v>
       </c>
-      <c r="J23" s="41">
+      <c r="J23" s="62">
         <v>245</v>
       </c>
-      <c r="K23" s="41">
+      <c r="K23" s="62">
         <v>28</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="37"/>
-      <c r="B24" s="43">
+      <c r="L23" s="59"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="58"/>
+      <c r="B24" s="65">
         <v>110118</v>
       </c>
-      <c r="C24" s="43">
+      <c r="C24" s="65">
         <v>99546</v>
       </c>
-      <c r="D24" s="43">
+      <c r="D24" s="65">
         <v>93632</v>
       </c>
-      <c r="E24" s="43">
+      <c r="E24" s="65">
         <v>96989</v>
       </c>
-      <c r="F24" s="43">
+      <c r="F24" s="65">
         <v>105313</v>
       </c>
-      <c r="G24" s="43">
+      <c r="G24" s="65">
         <v>123261</v>
       </c>
-      <c r="H24" s="43">
+      <c r="H24" s="65">
         <v>131919</v>
       </c>
-      <c r="I24" s="43">
+      <c r="I24" s="65">
         <v>148713</v>
       </c>
-      <c r="J24" s="43">
+      <c r="J24" s="65">
         <v>115391</v>
       </c>
-      <c r="K24" s="43">
+      <c r="K24" s="65">
         <v>108176</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="41" t="s">
+      <c r="L24" s="59"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" s="62" t="s">
         <v>92</v>
       </c>
-      <c r="B25" s="40">
+      <c r="B25" s="65">
         <v>3291</v>
       </c>
-      <c r="C25" s="41">
+      <c r="C25" s="62">
         <v>268</v>
       </c>
-      <c r="D25" s="41">
+      <c r="D25" s="62">
         <v>610</v>
       </c>
-      <c r="E25" s="41">
+      <c r="E25" s="62">
         <v>613</v>
       </c>
-      <c r="F25" s="41">
+      <c r="F25" s="62">
         <v>480</v>
       </c>
-      <c r="G25" s="41">
+      <c r="G25" s="62">
         <v>380</v>
       </c>
-      <c r="H25" s="41">
+      <c r="H25" s="62">
         <v>351</v>
       </c>
-      <c r="I25" s="41">
+      <c r="I25" s="62">
         <v>295</v>
       </c>
-      <c r="J25" s="41">
+      <c r="J25" s="62">
         <v>224</v>
       </c>
-      <c r="K25" s="41">
+      <c r="K25" s="62">
         <v>70</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="37"/>
-      <c r="B26" s="43">
+      <c r="L25" s="59"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" s="58"/>
+      <c r="B26" s="65">
         <v>127389</v>
       </c>
-      <c r="C26" s="43">
+      <c r="C26" s="65">
         <v>109046</v>
       </c>
-      <c r="D26" s="43">
+      <c r="D26" s="65">
         <v>100493</v>
       </c>
-      <c r="E26" s="43">
+      <c r="E26" s="65">
         <v>111602</v>
       </c>
-      <c r="F26" s="43">
+      <c r="F26" s="65">
         <v>112632</v>
       </c>
-      <c r="G26" s="43">
+      <c r="G26" s="65">
         <v>134768</v>
       </c>
-      <c r="H26" s="43">
+      <c r="H26" s="65">
         <v>147005</v>
       </c>
-      <c r="I26" s="43">
+      <c r="I26" s="65">
         <v>167347</v>
       </c>
-      <c r="J26" s="43">
+      <c r="J26" s="65">
         <v>186061</v>
       </c>
-      <c r="K26" s="43">
+      <c r="K26" s="65">
         <v>176875</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="38" t="s">
+      <c r="L26" s="59"/>
+    </row>
+    <row r="27" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="58" t="s">
         <v>93</v>
       </c>
-      <c r="B27" s="40">
+      <c r="B27" s="65">
         <v>1337</v>
       </c>
-      <c r="C27" s="41">
+      <c r="C27" s="62">
         <v>132</v>
       </c>
-      <c r="D27" s="41">
+      <c r="D27" s="62">
         <v>164</v>
       </c>
-      <c r="E27" s="41">
+      <c r="E27" s="62">
         <v>172</v>
       </c>
-      <c r="F27" s="41">
+      <c r="F27" s="62">
         <v>141</v>
       </c>
-      <c r="G27" s="41">
+      <c r="G27" s="62">
         <v>121</v>
       </c>
-      <c r="H27" s="41">
+      <c r="H27" s="62">
         <v>133</v>
       </c>
-      <c r="I27" s="41">
+      <c r="I27" s="62">
         <v>115</v>
       </c>
-      <c r="J27" s="41">
+      <c r="J27" s="62">
         <v>141</v>
       </c>
-      <c r="K27" s="41">
+      <c r="K27" s="62">
         <v>218</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="37"/>
-      <c r="B28" s="43">
+      <c r="L27" s="59"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="58"/>
+      <c r="B28" s="65">
         <v>163387</v>
       </c>
-      <c r="C28" s="43">
+      <c r="C28" s="65">
         <v>120037</v>
       </c>
-      <c r="D28" s="43">
+      <c r="D28" s="65">
         <v>120246</v>
       </c>
-      <c r="E28" s="43">
+      <c r="E28" s="65">
         <v>133740</v>
       </c>
-      <c r="F28" s="43">
+      <c r="F28" s="65">
         <v>152829</v>
       </c>
-      <c r="G28" s="43">
+      <c r="G28" s="65">
         <v>158421</v>
       </c>
-      <c r="H28" s="43">
+      <c r="H28" s="65">
         <v>182235</v>
       </c>
-      <c r="I28" s="43">
+      <c r="I28" s="65">
         <v>198905</v>
       </c>
-      <c r="J28" s="43">
+      <c r="J28" s="65">
         <v>201823</v>
       </c>
-      <c r="K28" s="43">
+      <c r="K28" s="65">
         <v>199972</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="38" t="s">
+      <c r="L28" s="59"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" s="58" t="s">
         <v>42</v>
       </c>
-      <c r="B29" s="40">
+      <c r="B29" s="65">
         <v>96278</v>
       </c>
-      <c r="C29" s="40">
+      <c r="C29" s="65">
         <v>22401</v>
       </c>
-      <c r="D29" s="40">
+      <c r="D29" s="65">
         <v>27903</v>
       </c>
-      <c r="E29" s="40">
+      <c r="E29" s="65">
         <v>19244</v>
       </c>
-      <c r="F29" s="40">
+      <c r="F29" s="65">
         <v>11568</v>
       </c>
-      <c r="G29" s="40">
+      <c r="G29" s="65">
         <v>6739</v>
       </c>
-      <c r="H29" s="40">
+      <c r="H29" s="65">
         <v>4967</v>
       </c>
-      <c r="I29" s="40">
+      <c r="I29" s="65">
         <v>2243</v>
       </c>
-      <c r="J29" s="41">
+      <c r="J29" s="62">
         <v>894</v>
       </c>
-      <c r="K29" s="41">
+      <c r="K29" s="62">
         <v>319</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="37"/>
-      <c r="B30" s="42">
+      <c r="L29" s="59"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" s="58"/>
+      <c r="B30" s="64">
         <v>94527</v>
       </c>
-      <c r="C30" s="42">
+      <c r="C30" s="64">
         <v>82337</v>
       </c>
-      <c r="D30" s="42">
+      <c r="D30" s="64">
         <v>88439</v>
       </c>
-      <c r="E30" s="42">
+      <c r="E30" s="64">
         <v>93978</v>
       </c>
-      <c r="F30" s="42">
+      <c r="F30" s="64">
         <v>101272</v>
       </c>
-      <c r="G30" s="42">
+      <c r="G30" s="64">
         <v>113443</v>
       </c>
-      <c r="H30" s="42">
+      <c r="H30" s="64">
         <v>115372</v>
       </c>
-      <c r="I30" s="42">
+      <c r="I30" s="64">
         <v>127861</v>
       </c>
-      <c r="J30" s="42">
+      <c r="J30" s="64">
         <v>139933</v>
       </c>
-      <c r="K30" s="42">
+      <c r="K30" s="64">
         <v>185781</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C31" s="49"/>
-      <c r="D31" s="49"/>
-      <c r="E31" s="49"/>
-      <c r="F31" s="49"/>
-      <c r="G31" s="49"/>
-      <c r="H31" s="49"/>
-      <c r="I31" s="49"/>
-      <c r="J31" s="49"/>
-      <c r="K31" s="49"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C32" s="49"/>
+      <c r="L30" s="59"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="59"/>
+      <c r="B31" s="59"/>
+      <c r="C31" s="66"/>
+      <c r="D31" s="66"/>
+      <c r="E31" s="66"/>
+      <c r="F31" s="66"/>
+      <c r="G31" s="66"/>
+      <c r="H31" s="66"/>
+      <c r="I31" s="66"/>
+      <c r="J31" s="66"/>
+      <c r="K31" s="66"/>
+      <c r="L31" s="59"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" s="59"/>
+      <c r="B32" s="59"/>
+      <c r="C32" s="66"/>
+      <c r="D32" s="59"/>
+      <c r="E32" s="59"/>
+      <c r="F32" s="59"/>
+      <c r="G32" s="59"/>
+      <c r="H32" s="59"/>
+      <c r="I32" s="59"/>
+      <c r="J32" s="59"/>
+      <c r="K32" s="59"/>
+      <c r="L32" s="59"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" s="59"/>
+      <c r="B33" s="59"/>
+      <c r="C33" s="59"/>
+      <c r="D33" s="59"/>
+      <c r="E33" s="59"/>
+      <c r="F33" s="59"/>
+      <c r="G33" s="59"/>
+      <c r="H33" s="59"/>
+      <c r="I33" s="59"/>
+      <c r="J33" s="59"/>
+      <c r="K33" s="59"/>
+      <c r="L33" s="59"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" s="59"/>
+      <c r="B34" s="59"/>
+      <c r="C34" s="59"/>
+      <c r="D34" s="59"/>
+      <c r="E34" s="59"/>
+      <c r="F34" s="59"/>
+      <c r="G34" s="59"/>
+      <c r="H34" s="59"/>
+      <c r="I34" s="59"/>
+      <c r="J34" s="59"/>
+      <c r="K34" s="59"/>
+      <c r="L34" s="59"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>